<commit_message>
Add demo code. Corrected a time issue in the logic. Added more test cases. Updated NuGet package
git-svn-id: https://solarcalculator.svn.codeplex.com/svn@26827 937343c3-697a-4e39-b5c6-83b50a1b7d63
</commit_message>
<xml_diff>
--- a/Source/Innovative.SolarCalculator.Tests/NOAA Solar Calculations Test Data.xlsx
+++ b/Source/Innovative.SolarCalculator.Tests/NOAA Solar Calculations Test Data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danie_000\Documents\Visual Studio 2012\Projects\CodePlex\solarcalculator\Source\Innovative.SolarCalculator.Tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danie_000\Documents\Visual Studio 2012\Projects\CodePlex TFS\solarcalculator\Source\Innovative.SolarCalculator.Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="339" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="339"/>
   </bookViews>
   <sheets>
     <sheet name="Calculations" sheetId="1" r:id="rId1"/>
@@ -611,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH2"/>
+  <dimension ref="A1:AH7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -883,6 +883,656 @@
         <v>357.32237072060843</v>
       </c>
     </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A3" s="15">
+        <v>35</v>
+      </c>
+      <c r="B3" s="15">
+        <v>-106</v>
+      </c>
+      <c r="C3" s="3">
+        <v>-7</v>
+      </c>
+      <c r="D3" s="2">
+        <v>41318</v>
+      </c>
+      <c r="E3" s="7">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="F3" s="9">
+        <f>D3+2415018.5+E3-C3/24</f>
+        <v>2456336.7923611109</v>
+      </c>
+      <c r="G3" s="9">
+        <f>(F3-2451545)/36525</f>
+        <v>0.13119212487641108</v>
+      </c>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9">
+        <f>MOD(280.46646+G3*(36000.76983 + G3*0.0003032),360)</f>
+        <v>323.48395640277977</v>
+      </c>
+      <c r="J3" s="9">
+        <f>357.52911+G3*(35999.05029 - 0.0001537*G3)</f>
+        <v>5080.3210084324937</v>
+      </c>
+      <c r="K3" s="9">
+        <f>0.016708634-G3*(0.000042037+0.0000001267*G3)</f>
+        <v>1.6703116895965531E-2</v>
+      </c>
+      <c r="L3" s="9">
+        <f>SIN(RADIANS(J3))*(1.914602-G3*(0.004817+0.000014*G3))+SIN(RADIANS(2*J3))*(0.019993-0.000101*G3)+SIN(RADIANS(3*J3))*0.000289</f>
+        <v>1.2584329274559338</v>
+      </c>
+      <c r="M3" s="9">
+        <f>I3+L3</f>
+        <v>324.74238933023571</v>
+      </c>
+      <c r="N3" s="9">
+        <f>J3+L3</f>
+        <v>5081.5794413599497</v>
+      </c>
+      <c r="O3" s="9">
+        <f>(1.000001018*(1-K3*K3))/(1+K3*COS(RADIANS(N3)))</f>
+        <v>0.98738510363968335</v>
+      </c>
+      <c r="P3" s="9">
+        <f>M3-0.00569-0.00478*SIN(RADIANS(125.04-1934.136*G3))</f>
+        <v>324.74042960961833</v>
+      </c>
+      <c r="Q3" s="9">
+        <f>23+(26+((21.448-G3*(46.815+G3*(0.00059-G3*0.001813))))/60)/60</f>
+        <v>23.437585065170264</v>
+      </c>
+      <c r="R3" s="9">
+        <f>Q3+0.00256*COS(RADIANS(125.04-1934.136*G3))</f>
+        <v>23.435984325009116</v>
+      </c>
+      <c r="S3" s="9">
+        <f>DEGREES(ATAN2(COS(RADIANS(P3)),COS(RADIANS(R3))*SIN(RADIANS(P3))))</f>
+        <v>-32.969791765354586</v>
+      </c>
+      <c r="T3" s="9">
+        <f>DEGREES(ASIN(SIN(RADIANS(R3))*SIN(RADIANS(P3))))</f>
+        <v>-13.273456138132213</v>
+      </c>
+      <c r="U3" s="9">
+        <f>TAN(RADIANS(R3/2))*TAN(RADIANS(R3/2))</f>
+        <v>4.3022042317213287E-2</v>
+      </c>
+      <c r="V3" s="9">
+        <f>4*DEGREES(U3*SIN(2*RADIANS(I3))-2*K3*SIN(RADIANS(J3))+4*K3*U3*SIN(RADIANS(J3))*COS(2*RADIANS(I3))-0.5*U3*U3*SIN(4*RADIANS(I3))-1.25*K3*K3*SIN(2*RADIANS(J3)))</f>
+        <v>-14.220819680016964</v>
+      </c>
+      <c r="W3" s="9">
+        <f>DEGREES(ACOS(COS(RADIANS(90.833))/(COS(RADIANS(A3))*COS(RADIANS(T3)))-TAN(RADIANS(A3))*TAN(RADIANS(T3))))</f>
+        <v>81.550090654441718</v>
+      </c>
+      <c r="X3" s="4">
+        <f>(720-4*B3-V3+C3*60)/1440</f>
+        <v>0.51265334700001186</v>
+      </c>
+      <c r="Y3" s="5">
+        <f>X3-W3*4/1440</f>
+        <v>0.28612531740434044</v>
+      </c>
+      <c r="Z3" s="5">
+        <f>X3+W3*4/1440</f>
+        <v>0.73918137659568328</v>
+      </c>
+      <c r="AA3" s="9">
+        <f>8*W3</f>
+        <v>652.40072523553374</v>
+      </c>
+      <c r="AB3" s="9">
+        <f>MOD(E3*1440+V3+4*B3-60*C3,1440)</f>
+        <v>1422.779180319983</v>
+      </c>
+      <c r="AC3" s="9">
+        <f>IF(AB3/4&lt;0,AB3/4+180,AB3/4-180)</f>
+        <v>175.69479507999574</v>
+      </c>
+      <c r="AD3" s="9">
+        <f>DEGREES(ACOS(SIN(RADIANS(A3))*SIN(RADIANS(T3))+COS(RADIANS(A3))*COS(RADIANS(T3))*COS(RADIANS(AC3))))</f>
+        <v>157.92787187499368</v>
+      </c>
+      <c r="AE3" s="9">
+        <f>90-AD3</f>
+        <v>-67.927871874993684</v>
+      </c>
+      <c r="AF3" s="9">
+        <f>IF(AE3&gt;85,0,IF(AE3&gt;5,58.1/TAN(RADIANS(AE3))-0.07/POWER(TAN(RADIANS(AE3)),3)+0.000086/POWER(TAN(RADIANS(AE3)),5),IF(AE3&gt;-0.575,1735+AE3*(-518.2+AE3*(103.4+AE3*(-12.79+AE3*0.711))),-20.772/TAN(RADIANS(AE3)))))/3600</f>
+        <v>2.3396850317577091E-3</v>
+      </c>
+      <c r="AG3" s="9">
+        <f>AE3+AF3</f>
+        <v>-67.925532189961928</v>
+      </c>
+      <c r="AH3" s="9">
+        <f>IF(AC3&gt;0,MOD(DEGREES(ACOS(((SIN(RADIANS(A3))*COS(RADIANS(AD3)))-SIN(RADIANS(T3)))/(COS(RADIANS(A3))*SIN(RADIANS(AD3)))))+180,360),MOD(540-DEGREES(ACOS(((SIN(RADIANS(A3))*COS(RADIANS(AD3)))-SIN(RADIANS(T3)))/(COS(RADIANS(#REF!))*SIN(RADIANS(AD3))))),360))</f>
+        <v>348.78822709328472</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A4" s="15">
+        <v>61</v>
+      </c>
+      <c r="B4" s="15">
+        <v>-149</v>
+      </c>
+      <c r="C4" s="3">
+        <v>-9</v>
+      </c>
+      <c r="D4" s="2">
+        <v>41318</v>
+      </c>
+      <c r="E4" s="7">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="F4" s="9">
+        <f t="shared" ref="F4:F7" si="0">D4+2415018.5+E4-C4/24</f>
+        <v>2456336.8756944444</v>
+      </c>
+      <c r="G4" s="9">
+        <f t="shared" ref="G4:G7" si="1">(F4-2451545)/36525</f>
+        <v>0.13119440641873795</v>
+      </c>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9">
+        <f t="shared" ref="I4:I7" si="2">MOD(280.46646+G4*(36000.76983 + G4*0.0003032),360)</f>
+        <v>323.5660936831282</v>
+      </c>
+      <c r="J4" s="9">
+        <f t="shared" ref="J4:J7" si="3">357.52911+G4*(35999.05029 - 0.0001537*G4)</f>
+        <v>5080.4031417893657</v>
+      </c>
+      <c r="K4" s="9">
+        <f t="shared" ref="K4:K7" si="4">0.016708634-G4*(0.000042037+0.0000001267*G4)</f>
+        <v>1.6703116799980489E-2</v>
+      </c>
+      <c r="L4" s="9">
+        <f t="shared" ref="L4:L7" si="5">SIN(RADIANS(J4))*(1.914602-G4*(0.004817+0.000014*G4))+SIN(RADIANS(2*J4))*(0.019993-0.000101*G4)+SIN(RADIANS(3*J4))*0.000289</f>
+        <v>1.2605320984406281</v>
+      </c>
+      <c r="M4" s="9">
+        <f t="shared" ref="M4:M7" si="6">I4+L4</f>
+        <v>324.82662578156885</v>
+      </c>
+      <c r="N4" s="9">
+        <f t="shared" ref="N4:N7" si="7">J4+L4</f>
+        <v>5081.663673887806</v>
+      </c>
+      <c r="O4" s="9">
+        <f t="shared" ref="O4:O7" si="8">(1.000001018*(1-K4*K4))/(1+K4*COS(RADIANS(N4)))</f>
+        <v>0.98740100965328081</v>
+      </c>
+      <c r="P4" s="9">
+        <f t="shared" ref="P4:P7" si="9">M4-0.00569-0.00478*SIN(RADIANS(125.04-1934.136*G4))</f>
+        <v>324.82466583074233</v>
+      </c>
+      <c r="Q4" s="9">
+        <f t="shared" ref="Q4:Q7" si="10">23+(26+((21.448-G4*(46.815+G4*(0.00059-G4*0.001813))))/60)/60</f>
+        <v>23.437585035500668</v>
+      </c>
+      <c r="R4" s="9">
+        <f t="shared" ref="R4:R7" si="11">Q4+0.00256*COS(RADIANS(125.04-1934.136*G4))</f>
+        <v>23.435984141476965</v>
+      </c>
+      <c r="S4" s="9">
+        <f t="shared" ref="S4:S7" si="12">DEGREES(ATAN2(COS(RADIANS(P4)),COS(RADIANS(R4))*SIN(RADIANS(P4))))</f>
+        <v>-32.888213113134071</v>
+      </c>
+      <c r="T4" s="9">
+        <f t="shared" ref="T4:T7" si="13">DEGREES(ASIN(SIN(RADIANS(R4))*SIN(RADIANS(P4))))</f>
+        <v>-13.24533565256583</v>
+      </c>
+      <c r="U4" s="9">
+        <f t="shared" ref="U4:U7" si="14">TAN(RADIANS(R4/2))*TAN(RADIANS(R4/2))</f>
+        <v>4.3022041624220804E-2</v>
+      </c>
+      <c r="V4" s="9">
+        <f t="shared" ref="V4:V7" si="15">4*DEGREES(U4*SIN(2*RADIANS(I4))-2*K4*SIN(RADIANS(J4))+4*K4*U4*SIN(RADIANS(J4))*COS(2*RADIANS(I4))-0.5*U4*U4*SIN(4*RADIANS(I4))-1.25*K4*K4*SIN(2*RADIANS(J4)))</f>
+        <v>-14.218542691518463</v>
+      </c>
+      <c r="W4" s="9">
+        <f t="shared" ref="W4:W7" si="16">DEGREES(ACOS(COS(RADIANS(90.833))/(COS(RADIANS(A4))*COS(RADIANS(T4)))-TAN(RADIANS(A4))*TAN(RADIANS(T4))))</f>
+        <v>66.806655732106847</v>
+      </c>
+      <c r="X4" s="4">
+        <f t="shared" ref="X4:X7" si="17">(720-4*B4-V4+C4*60)/1440</f>
+        <v>0.54876287686911007</v>
+      </c>
+      <c r="Y4" s="5">
+        <f t="shared" ref="Y4:Y7" si="18">X4-W4*4/1440</f>
+        <v>0.36318883316881329</v>
+      </c>
+      <c r="Z4" s="5">
+        <f t="shared" ref="Z4:Z7" si="19">X4+W4*4/1440</f>
+        <v>0.7343369205694068</v>
+      </c>
+      <c r="AA4" s="9">
+        <f t="shared" ref="AA4:AA7" si="20">8*W4</f>
+        <v>534.45324585685478</v>
+      </c>
+      <c r="AB4" s="9">
+        <f t="shared" ref="AB4:AB7" si="21">MOD(E4*1440+V4+4*B4-60*C4,1440)</f>
+        <v>1370.7814573084815</v>
+      </c>
+      <c r="AC4" s="9">
+        <f t="shared" ref="AC4:AC7" si="22">IF(AB4/4&lt;0,AB4/4+180,AB4/4-180)</f>
+        <v>162.69536432712039</v>
+      </c>
+      <c r="AD4" s="9">
+        <f t="shared" ref="AD4:AD7" si="23">DEGREES(ACOS(SIN(RADIANS(A4))*SIN(RADIANS(T4))+COS(RADIANS(A4))*COS(RADIANS(T4))*COS(RADIANS(AC4))))</f>
+        <v>130.61298218479848</v>
+      </c>
+      <c r="AE4" s="9">
+        <f t="shared" ref="AE4:AE7" si="24">90-AD4</f>
+        <v>-40.612982184798483</v>
+      </c>
+      <c r="AF4" s="9">
+        <f t="shared" ref="AF4:AF7" si="25">IF(AE4&gt;85,0,IF(AE4&gt;5,58.1/TAN(RADIANS(AE4))-0.07/POWER(TAN(RADIANS(AE4)),3)+0.000086/POWER(TAN(RADIANS(AE4)),5),IF(AE4&gt;-0.575,1735+AE4*(-518.2+AE4*(103.4+AE4*(-12.79+AE4*0.711))),-20.772/TAN(RADIANS(AE4)))))/3600</f>
+        <v>6.7288883012048394E-3</v>
+      </c>
+      <c r="AG4" s="9">
+        <f t="shared" ref="AG4:AG7" si="26">AE4+AF4</f>
+        <v>-40.606253296497279</v>
+      </c>
+      <c r="AH4" s="9">
+        <f>IF(AC4&gt;0,MOD(DEGREES(ACOS(((SIN(RADIANS(A4))*COS(RADIANS(AD4)))-SIN(RADIANS(T4)))/(COS(RADIANS(A4))*SIN(RADIANS(AD4)))))+180,360),MOD(540-DEGREES(ACOS(((SIN(RADIANS(A4))*COS(RADIANS(AD4)))-SIN(RADIANS(T4)))/(COS(RADIANS(#REF!))*SIN(RADIANS(AD4))))),360))</f>
+        <v>337.57880009155303</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A5" s="15">
+        <v>33</v>
+      </c>
+      <c r="B5" s="15">
+        <v>-84</v>
+      </c>
+      <c r="C5" s="3">
+        <v>-5</v>
+      </c>
+      <c r="D5" s="2">
+        <v>41318</v>
+      </c>
+      <c r="E5" s="7">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="F5" s="9">
+        <f t="shared" si="0"/>
+        <v>2456336.7090277779</v>
+      </c>
+      <c r="G5" s="9">
+        <f t="shared" si="1"/>
+        <v>0.13118984333409697</v>
+      </c>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9">
+        <f t="shared" si="2"/>
+        <v>323.40181912289063</v>
+      </c>
+      <c r="J5" s="9">
+        <f t="shared" si="3"/>
+        <v>5080.2388750760829</v>
+      </c>
+      <c r="K5" s="9">
+        <f t="shared" si="4"/>
+        <v>1.6703116991950574E-2</v>
+      </c>
+      <c r="L5" s="9">
+        <f t="shared" si="5"/>
+        <v>1.2563310448816958</v>
+      </c>
+      <c r="M5" s="9">
+        <f t="shared" si="6"/>
+        <v>324.65815016777231</v>
+      </c>
+      <c r="N5" s="9">
+        <f t="shared" si="7"/>
+        <v>5081.4952061209642</v>
+      </c>
+      <c r="O5" s="9">
+        <f t="shared" si="8"/>
+        <v>0.9873692239615508</v>
+      </c>
+      <c r="P5" s="9">
+        <f t="shared" si="9"/>
+        <v>324.65619067734195</v>
+      </c>
+      <c r="Q5" s="9">
+        <f t="shared" si="10"/>
+        <v>23.437585094839857</v>
+      </c>
+      <c r="R5" s="9">
+        <f t="shared" si="11"/>
+        <v>23.435984508550757</v>
+      </c>
+      <c r="S5" s="9">
+        <f t="shared" si="12"/>
+        <v>-33.05139192760052</v>
+      </c>
+      <c r="T5" s="9">
+        <f t="shared" si="13"/>
+        <v>-13.301551565764298</v>
+      </c>
+      <c r="U5" s="9">
+        <f t="shared" si="14"/>
+        <v>4.3022043010241588E-2</v>
+      </c>
+      <c r="V5" s="9">
+        <f t="shared" si="15"/>
+        <v>-14.223009538608482</v>
+      </c>
+      <c r="W5" s="9">
+        <f t="shared" si="16"/>
+        <v>82.199773916850745</v>
+      </c>
+      <c r="X5" s="4">
+        <f t="shared" si="17"/>
+        <v>0.53487708995736705</v>
+      </c>
+      <c r="Y5" s="5">
+        <f t="shared" si="18"/>
+        <v>0.30654438463278166</v>
+      </c>
+      <c r="Z5" s="5">
+        <f t="shared" si="19"/>
+        <v>0.76320979528195243</v>
+      </c>
+      <c r="AA5" s="9">
+        <f t="shared" si="20"/>
+        <v>657.59819133480596</v>
+      </c>
+      <c r="AB5" s="9">
+        <f t="shared" si="21"/>
+        <v>1390.7769904613915</v>
+      </c>
+      <c r="AC5" s="9">
+        <f t="shared" si="22"/>
+        <v>167.69424761534788</v>
+      </c>
+      <c r="AD5" s="9">
+        <f t="shared" si="23"/>
+        <v>157.32813407708417</v>
+      </c>
+      <c r="AE5" s="9">
+        <f t="shared" si="24"/>
+        <v>-67.328134077084172</v>
+      </c>
+      <c r="AF5" s="9">
+        <f t="shared" si="25"/>
+        <v>2.4103149413600175E-3</v>
+      </c>
+      <c r="AG5" s="9">
+        <f t="shared" si="26"/>
+        <v>-67.325723762142815</v>
+      </c>
+      <c r="AH5" s="9">
+        <f>IF(AC5&gt;0,MOD(DEGREES(ACOS(((SIN(RADIANS(A5))*COS(RADIANS(AD5)))-SIN(RADIANS(T5)))/(COS(RADIANS(A5))*SIN(RADIANS(AD5)))))+180,360),MOD(540-DEGREES(ACOS(((SIN(RADIANS(A5))*COS(RADIANS(AD5)))-SIN(RADIANS(T5)))/(COS(RADIANS(#REF!))*SIN(RADIANS(AD5))))),360))</f>
+        <v>327.44586544226365</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A6" s="15">
+        <v>30</v>
+      </c>
+      <c r="B6" s="15">
+        <v>97</v>
+      </c>
+      <c r="C6" s="3">
+        <v>-6</v>
+      </c>
+      <c r="D6" s="2">
+        <v>41318</v>
+      </c>
+      <c r="E6" s="7">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="F6" s="9">
+        <f t="shared" si="0"/>
+        <v>2456336.7506944444</v>
+      </c>
+      <c r="G6" s="9">
+        <f t="shared" si="1"/>
+        <v>0.13119098410525401</v>
+      </c>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9">
+        <f t="shared" si="2"/>
+        <v>323.4428877628352</v>
+      </c>
+      <c r="J6" s="9">
+        <f t="shared" si="3"/>
+        <v>5080.2799417542874</v>
+      </c>
+      <c r="K6" s="9">
+        <f t="shared" si="4"/>
+        <v>1.6703116943958051E-2</v>
+      </c>
+      <c r="L6" s="9">
+        <f t="shared" si="5"/>
+        <v>1.2573823248461911</v>
+      </c>
+      <c r="M6" s="9">
+        <f t="shared" si="6"/>
+        <v>324.70027008768142</v>
+      </c>
+      <c r="N6" s="9">
+        <f t="shared" si="7"/>
+        <v>5081.5373240791332</v>
+      </c>
+      <c r="O6" s="9">
+        <f t="shared" si="8"/>
+        <v>0.98737716050649549</v>
+      </c>
+      <c r="P6" s="9">
+        <f t="shared" si="9"/>
+        <v>324.69831048216031</v>
+      </c>
+      <c r="Q6" s="9">
+        <f t="shared" si="10"/>
+        <v>23.437585080005061</v>
+      </c>
+      <c r="R6" s="9">
+        <f t="shared" si="11"/>
+        <v>23.435984416778748</v>
+      </c>
+      <c r="S6" s="9">
+        <f t="shared" si="12"/>
+        <v>-33.010589156044496</v>
+      </c>
+      <c r="T6" s="9">
+        <f t="shared" si="13"/>
+        <v>-13.287506988356013</v>
+      </c>
+      <c r="U6" s="9">
+        <f t="shared" si="14"/>
+        <v>4.3022042663722941E-2</v>
+      </c>
+      <c r="V6" s="9">
+        <f t="shared" si="15"/>
+        <v>-14.221925507165402</v>
+      </c>
+      <c r="W6" s="9">
+        <f t="shared" si="16"/>
+        <v>83.159951233929917</v>
+      </c>
+      <c r="X6" s="4">
+        <f t="shared" si="17"/>
+        <v>-9.5681072866906983E-3</v>
+      </c>
+      <c r="Y6" s="5">
+        <f t="shared" si="18"/>
+        <v>-0.24056797182538489</v>
+      </c>
+      <c r="Z6" s="5">
+        <f t="shared" si="19"/>
+        <v>0.22143175725200351</v>
+      </c>
+      <c r="AA6" s="9">
+        <f t="shared" si="20"/>
+        <v>665.27960987143933</v>
+      </c>
+      <c r="AB6" s="9">
+        <f t="shared" si="21"/>
+        <v>734.77807449283455</v>
+      </c>
+      <c r="AC6" s="9">
+        <f t="shared" si="22"/>
+        <v>3.6945186232086371</v>
+      </c>
+      <c r="AD6" s="9">
+        <f t="shared" si="23"/>
+        <v>43.43367839837498</v>
+      </c>
+      <c r="AE6" s="9">
+        <f t="shared" si="24"/>
+        <v>46.56632160162502</v>
+      </c>
+      <c r="AF6" s="9">
+        <f t="shared" si="25"/>
+        <v>1.526328490540226E-2</v>
+      </c>
+      <c r="AG6" s="9">
+        <f t="shared" si="26"/>
+        <v>46.581584886530422</v>
+      </c>
+      <c r="AH6" s="9">
+        <f>IF(AC6&gt;0,MOD(DEGREES(ACOS(((SIN(RADIANS(A6))*COS(RADIANS(AD6)))-SIN(RADIANS(T6)))/(COS(RADIANS(A6))*SIN(RADIANS(AD6)))))+180,360),MOD(540-DEGREES(ACOS(((SIN(RADIANS(A6))*COS(RADIANS(AD6)))-SIN(RADIANS(T6)))/(COS(RADIANS(#REF!))*SIN(RADIANS(AD6))))),360))</f>
+        <v>185.23352312257745</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A7" s="15">
+        <v>33</v>
+      </c>
+      <c r="B7" s="15">
+        <v>-86</v>
+      </c>
+      <c r="C7" s="3">
+        <v>-6</v>
+      </c>
+      <c r="D7" s="2">
+        <v>41318</v>
+      </c>
+      <c r="E7" s="7">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="F7" s="9">
+        <f t="shared" si="0"/>
+        <v>2456336.7506944444</v>
+      </c>
+      <c r="G7" s="9">
+        <f t="shared" si="1"/>
+        <v>0.13119098410525401</v>
+      </c>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9">
+        <f t="shared" si="2"/>
+        <v>323.4428877628352</v>
+      </c>
+      <c r="J7" s="9">
+        <f t="shared" si="3"/>
+        <v>5080.2799417542874</v>
+      </c>
+      <c r="K7" s="9">
+        <f t="shared" si="4"/>
+        <v>1.6703116943958051E-2</v>
+      </c>
+      <c r="L7" s="9">
+        <f t="shared" si="5"/>
+        <v>1.2573823248461911</v>
+      </c>
+      <c r="M7" s="9">
+        <f t="shared" si="6"/>
+        <v>324.70027008768142</v>
+      </c>
+      <c r="N7" s="9">
+        <f t="shared" si="7"/>
+        <v>5081.5373240791332</v>
+      </c>
+      <c r="O7" s="9">
+        <f t="shared" si="8"/>
+        <v>0.98737716050649549</v>
+      </c>
+      <c r="P7" s="9">
+        <f t="shared" si="9"/>
+        <v>324.69831048216031</v>
+      </c>
+      <c r="Q7" s="9">
+        <f t="shared" si="10"/>
+        <v>23.437585080005061</v>
+      </c>
+      <c r="R7" s="9">
+        <f t="shared" si="11"/>
+        <v>23.435984416778748</v>
+      </c>
+      <c r="S7" s="9">
+        <f t="shared" si="12"/>
+        <v>-33.010589156044496</v>
+      </c>
+      <c r="T7" s="9">
+        <f t="shared" si="13"/>
+        <v>-13.287506988356013</v>
+      </c>
+      <c r="U7" s="9">
+        <f t="shared" si="14"/>
+        <v>4.3022042663722941E-2</v>
+      </c>
+      <c r="V7" s="9">
+        <f t="shared" si="15"/>
+        <v>-14.221925507165402</v>
+      </c>
+      <c r="W7" s="9">
+        <f t="shared" si="16"/>
+        <v>82.209433962078904</v>
+      </c>
+      <c r="X7" s="4">
+        <f t="shared" si="17"/>
+        <v>0.4987652260466427</v>
+      </c>
+      <c r="Y7" s="5">
+        <f t="shared" si="18"/>
+        <v>0.27040568726309022</v>
+      </c>
+      <c r="Z7" s="5">
+        <f t="shared" si="19"/>
+        <v>0.72712476483019517</v>
+      </c>
+      <c r="AA7" s="9">
+        <f t="shared" si="20"/>
+        <v>657.67547169663123</v>
+      </c>
+      <c r="AB7" s="9">
+        <f t="shared" si="21"/>
+        <v>2.7780744928346053</v>
+      </c>
+      <c r="AC7" s="9">
+        <f t="shared" si="22"/>
+        <v>-179.30548137679136</v>
+      </c>
+      <c r="AD7" s="9">
+        <f t="shared" si="23"/>
+        <v>160.27732361733925</v>
+      </c>
+      <c r="AE7" s="9">
+        <f t="shared" si="24"/>
+        <v>-70.277323617339249</v>
+      </c>
+      <c r="AF7" s="9">
+        <f t="shared" si="25"/>
+        <v>2.0685358681994024E-3</v>
+      </c>
+      <c r="AG7" s="9">
+        <f t="shared" si="26"/>
+        <v>-70.275255081471045</v>
+      </c>
+      <c r="AH7" s="9" t="e">
+        <f>IF(AC7&gt;0,MOD(DEGREES(ACOS(((SIN(RADIANS(A7))*COS(RADIANS(AD7)))-SIN(RADIANS(T7)))/(COS(RADIANS(A7))*SIN(RADIANS(AD7)))))+180,360),MOD(540-DEGREES(ACOS(((SIN(RADIANS(A7))*COS(RADIANS(AD7)))-SIN(RADIANS(T7)))/(COS(RADIANS(#REF!))*SIN(RADIANS(AD7))))),360))</f>
+        <v>#REF!</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -893,7 +1543,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -949,23 +1599,23 @@
     <row r="2" spans="1:11" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A2" s="16">
         <f ca="1">RANDBETWEEN(1,360)</f>
-        <v>273</v>
+        <v>196</v>
       </c>
       <c r="B2" s="16">
         <f ca="1">RANDBETWEEN(1,5)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C2" s="17">
         <f ca="1">RANDBETWEEN(0,2*PI()) + (RANDBETWEEN(0,10000000000000000000)/10000000000000000000)</f>
-        <v>0.8481272416039074</v>
+        <v>3.5495762538318352</v>
       </c>
       <c r="D2" s="17">
         <f ca="1">RADIANS(A2)</f>
-        <v>4.7647488579445199</v>
+        <v>3.4208453339088858</v>
       </c>
       <c r="E2" s="17">
         <f ca="1">DEGREES(C2)</f>
-        <v>48.594111433976181</v>
+        <v>203.37573840442155</v>
       </c>
       <c r="F2" s="16">
         <f t="shared" ref="F2:F21" ca="1" si="0">MOD(A2,B2)</f>
@@ -973,121 +1623,121 @@
       </c>
       <c r="G2" s="17">
         <f ca="1">SIN(A2)</f>
-        <v>0.31320015487066988</v>
+        <v>0.9395300555699313</v>
       </c>
       <c r="H2" s="17">
         <f ca="1">ASIN(G2)</f>
-        <v>0.31856086231201175</v>
+        <v>1.221255477432819</v>
       </c>
       <c r="I2" s="17">
         <f t="shared" ref="I2:I21" ca="1" si="1">COS(A2)</f>
-        <v>-0.9496871395301657</v>
+        <v>0.34246645774551659</v>
       </c>
       <c r="J2" s="17">
         <f ca="1">ACOS(I2)</f>
-        <v>2.8230317912777814</v>
+        <v>1.2212554774328193</v>
       </c>
       <c r="K2" s="17">
         <f ca="1">TAN(A2)</f>
-        <v>-0.32979298321931361</v>
+        <v>2.7434221200958802</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A3" s="16">
         <f t="shared" ref="A3:A21" ca="1" si="2">RANDBETWEEN(1,360)</f>
-        <v>210</v>
+        <v>177</v>
       </c>
       <c r="B3" s="16">
         <f t="shared" ref="B3:B21" ca="1" si="3">RANDBETWEEN(1,5)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3" s="17">
         <f ca="1">RANDBETWEEN(0,2*PI()) + (RANDBETWEEN(0,10000000000000000000)/10000000000000000000)</f>
-        <v>3.433889971408715</v>
+        <v>4.6678910745942579</v>
       </c>
       <c r="D3" s="17">
         <f t="shared" ref="D3:D21" ca="1" si="4">RADIANS(A3)</f>
-        <v>3.6651914291880923</v>
+        <v>3.0892327760299634</v>
       </c>
       <c r="E3" s="17">
         <f t="shared" ref="E3:E21" ca="1" si="5">DEGREES(C3)</f>
-        <v>196.7474026740183</v>
+        <v>267.45045780103749</v>
       </c>
       <c r="F3" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" s="17">
         <f t="shared" ref="G3:G21" ca="1" si="6">SIN(A3)</f>
-        <v>0.46771851834275896</v>
+        <v>0.87758978777711572</v>
       </c>
       <c r="H3" s="17">
         <f t="shared" ref="H3:H21" ca="1" si="7">ASIN(G3)</f>
-        <v>0.48670779051614704</v>
+        <v>1.0708113989715786</v>
       </c>
       <c r="I3" s="17">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.88387747318237175</v>
+        <v>0.47941231147032193</v>
       </c>
       <c r="J3" s="17">
         <f t="shared" ref="J3:J21" ca="1" si="8">ACOS(I3)</f>
-        <v>2.6548848630736464</v>
+        <v>1.0708113989715786</v>
       </c>
       <c r="K3" s="17">
         <f t="shared" ref="K3:K21" ca="1" si="9">TAN(A3)</f>
-        <v>-0.5291666916894644</v>
+        <v>1.8305532978191841</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A4" s="16">
         <f t="shared" ca="1" si="2"/>
-        <v>23</v>
+        <v>299</v>
       </c>
       <c r="B4" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C4" s="17">
         <f t="shared" ref="C4:C21" ca="1" si="10">RANDBETWEEN(0,2*PI()) + (RANDBETWEEN(0,10000000000000000000)/10000000000000000000)</f>
-        <v>6.2649390130595455</v>
+        <v>2.2773962752671175</v>
       </c>
       <c r="D4" s="17">
         <f t="shared" ca="1" si="4"/>
-        <v>0.4014257279586958</v>
+        <v>5.2185344634630457</v>
       </c>
       <c r="E4" s="17">
         <f t="shared" ca="1" si="5"/>
-        <v>358.95456435516729</v>
+        <v>130.4851948516197</v>
       </c>
       <c r="F4" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G4" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>-0.84622040417517064</v>
+        <v>-0.52157672161837043</v>
       </c>
       <c r="H4" s="17">
         <f t="shared" ca="1" si="7"/>
-        <v>-1.0088514248714473</v>
+        <v>-0.54869790896964232</v>
       </c>
       <c r="I4" s="17">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.53283302033339752</v>
+        <v>-0.85320438551722932</v>
       </c>
       <c r="J4" s="17">
         <f t="shared" ca="1" si="8"/>
-        <v>2.1327412287183458</v>
+        <v>2.5928947446201507</v>
       </c>
       <c r="K4" s="17">
         <f t="shared" ca="1" si="9"/>
-        <v>1.5881530833912738</v>
+        <v>0.61131509691218988</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A5" s="16">
         <f t="shared" ca="1" si="2"/>
-        <v>288</v>
+        <v>66</v>
       </c>
       <c r="B5" s="16">
         <f t="shared" ca="1" si="3"/>
@@ -1095,15 +1745,15 @@
       </c>
       <c r="C5" s="17">
         <f t="shared" ca="1" si="10"/>
-        <v>2.2895387081774605</v>
+        <v>6.4246288284769291</v>
       </c>
       <c r="D5" s="17">
         <f t="shared" ca="1" si="4"/>
-        <v>5.026548245743669</v>
+        <v>1.1519173063162575</v>
       </c>
       <c r="E5" s="17">
         <f t="shared" ca="1" si="5"/>
-        <v>131.18090501040311</v>
+        <v>368.1041168098065</v>
       </c>
       <c r="F5" s="16">
         <f t="shared" ca="1" si="0"/>
@@ -1111,137 +1761,137 @@
       </c>
       <c r="G5" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>-0.85550437075082075</v>
+        <v>-2.6551154023966794E-2</v>
       </c>
       <c r="H5" s="17">
         <f t="shared" ca="1" si="7"/>
-        <v>-1.026524130260978</v>
+        <v>-2.655427461434199E-2</v>
       </c>
       <c r="I5" s="17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.51779558865081332</v>
+        <v>-0.99964745596634996</v>
       </c>
       <c r="J5" s="17">
         <f t="shared" ca="1" si="8"/>
-        <v>1.0265241302609778</v>
+        <v>3.1150383789754512</v>
       </c>
       <c r="K5" s="17">
         <f t="shared" ca="1" si="9"/>
-        <v>-1.6522048265802214</v>
+        <v>2.6560517776039391E-2</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A6" s="16">
         <f t="shared" ca="1" si="2"/>
-        <v>273</v>
+        <v>78</v>
       </c>
       <c r="B6" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" s="17">
         <f t="shared" ca="1" si="10"/>
-        <v>2.8645792399344301</v>
+        <v>6.0149327351138364</v>
       </c>
       <c r="D6" s="17">
         <f t="shared" ca="1" si="4"/>
-        <v>4.7647488579445199</v>
+        <v>1.3613568165555769</v>
       </c>
       <c r="E6" s="17">
         <f t="shared" ca="1" si="5"/>
-        <v>164.12830052903604</v>
+        <v>344.63025977710356</v>
       </c>
       <c r="F6" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>0.31320015487066988</v>
+        <v>0.51397845598753522</v>
       </c>
       <c r="H6" s="17">
         <f t="shared" ca="1" si="7"/>
-        <v>0.31856086231201175</v>
+        <v>0.53981633974483101</v>
       </c>
       <c r="I6" s="17">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.9496871395301657</v>
+        <v>-0.85780309324498782</v>
       </c>
       <c r="J6" s="17">
         <f t="shared" ca="1" si="8"/>
-        <v>2.8230317912777814</v>
+        <v>2.6017763138449621</v>
       </c>
       <c r="K6" s="17">
         <f t="shared" ca="1" si="9"/>
-        <v>-0.32979298321931361</v>
+        <v>-0.59917999834111513</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A7" s="16">
         <f t="shared" ca="1" si="2"/>
-        <v>145</v>
+        <v>49</v>
       </c>
       <c r="B7" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C7" s="17">
         <f t="shared" ca="1" si="10"/>
-        <v>6.5108232405624955</v>
+        <v>0.80399022653808361</v>
       </c>
       <c r="D7" s="17">
         <f t="shared" ca="1" si="4"/>
-        <v>2.530727415391778</v>
+        <v>0.85521133347722145</v>
       </c>
       <c r="E7" s="17">
         <f t="shared" ca="1" si="5"/>
-        <v>373.0426928399209</v>
+        <v>46.065246750399147</v>
       </c>
       <c r="F7" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>0.46774516204513333</v>
+        <v>-0.95375265275947185</v>
       </c>
       <c r="H7" s="17">
         <f t="shared" ca="1" si="7"/>
-        <v>0.486737934869511</v>
+        <v>-1.2654824574366923</v>
       </c>
       <c r="I7" s="17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.88386337370850021</v>
+        <v>0.30059254374363709</v>
       </c>
       <c r="J7" s="17">
         <f t="shared" ca="1" si="8"/>
-        <v>0.48673793486951111</v>
+        <v>1.2654824574366916</v>
       </c>
       <c r="K7" s="17">
         <f t="shared" ca="1" si="9"/>
-        <v>0.52920527760141867</v>
+        <v>-3.1729085521591909</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A8" s="16">
         <f t="shared" ca="1" si="2"/>
-        <v>259</v>
+        <v>228</v>
       </c>
       <c r="B8" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C8" s="17">
         <f t="shared" ca="1" si="10"/>
-        <v>2.8575456462563427</v>
+        <v>2.7416258847965862</v>
       </c>
       <c r="D8" s="17">
         <f t="shared" ca="1" si="4"/>
-        <v>4.5204027626653138</v>
+        <v>3.9793506945470716</v>
       </c>
       <c r="E8" s="17">
         <f t="shared" ca="1" si="5"/>
-        <v>163.72530529647173</v>
+        <v>157.08359220266445</v>
       </c>
       <c r="F8" s="16">
         <f t="shared" ca="1" si="0"/>
@@ -1249,137 +1899,137 @@
       </c>
       <c r="G8" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>0.98359318394668083</v>
+        <v>0.97262306248562436</v>
       </c>
       <c r="H8" s="17">
         <f t="shared" ca="1" si="7"/>
-        <v>1.3894024056369543</v>
+        <v>1.3362637120549066</v>
       </c>
       <c r="I8" s="17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.18040079959254857</v>
+        <v>-0.23238842122852266</v>
       </c>
       <c r="J8" s="17">
         <f t="shared" ca="1" si="8"/>
-        <v>1.3894024056369543</v>
+        <v>1.8053289415348868</v>
       </c>
       <c r="K8" s="17">
         <f t="shared" ca="1" si="9"/>
-        <v>5.4522662103949351</v>
+        <v>-4.1853335779117016</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
         <f t="shared" ca="1" si="2"/>
-        <v>26</v>
+        <v>183</v>
       </c>
       <c r="B9" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" s="17">
         <f t="shared" ca="1" si="10"/>
-        <v>5.79543719646969</v>
+        <v>3.9831460364895257</v>
       </c>
       <c r="D9" s="17">
         <f t="shared" ca="1" si="4"/>
-        <v>0.4537856055185257</v>
+        <v>3.1939525311496229</v>
       </c>
       <c r="E9" s="17">
         <f t="shared" ca="1" si="5"/>
-        <v>332.0540917908433</v>
+        <v>228.21745707511161</v>
       </c>
       <c r="F9" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>0.76255845047960269</v>
+        <v>0.70868040823920841</v>
       </c>
       <c r="H9" s="17">
         <f t="shared" ca="1" si="7"/>
-        <v>0.86725877128165396</v>
+        <v>0.78762609179199206</v>
       </c>
       <c r="I9" s="17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.64691932232864036</v>
+        <v>0.70552964429420606</v>
       </c>
       <c r="J9" s="17">
         <f t="shared" ca="1" si="8"/>
-        <v>0.86725877128165396</v>
+        <v>0.78762609179199194</v>
       </c>
       <c r="K9" s="17">
         <f t="shared" ca="1" si="9"/>
-        <v>1.1787535542062797</v>
+        <v>1.0044658136911517</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A10" s="16">
         <f t="shared" ca="1" si="2"/>
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B10" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" s="17">
         <f t="shared" ca="1" si="10"/>
-        <v>4.3151516784748924</v>
+        <v>6.6962389596994871</v>
       </c>
       <c r="D10" s="17">
         <f t="shared" ca="1" si="4"/>
-        <v>1.1170107212763709</v>
+        <v>1.1693705988362009</v>
       </c>
       <c r="E10" s="17">
         <f t="shared" ca="1" si="5"/>
-        <v>247.23997913540455</v>
+        <v>383.66623100185359</v>
       </c>
       <c r="F10" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G10" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>0.92002603819679063</v>
+        <v>-0.85551997897532228</v>
       </c>
       <c r="H10" s="17">
         <f t="shared" ca="1" si="7"/>
-        <v>1.168146928204135</v>
+        <v>-1.0265542746143421</v>
       </c>
       <c r="I10" s="17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.39185723042955001</v>
+        <v>-0.5177697997895051</v>
       </c>
       <c r="J10" s="17">
         <f t="shared" ca="1" si="8"/>
-        <v>1.168146928204135</v>
+        <v>2.1150383789754512</v>
       </c>
       <c r="K10" s="17">
         <f t="shared" ca="1" si="9"/>
-        <v>2.3478603091954366</v>
+        <v>1.6523172640102353</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A11" s="16">
         <f t="shared" ca="1" si="2"/>
-        <v>158</v>
+        <v>228</v>
       </c>
       <c r="B11" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11" s="17">
         <f t="shared" ca="1" si="10"/>
-        <v>4.4410329475985506</v>
+        <v>4.7205144751909351</v>
       </c>
       <c r="D11" s="17">
         <f t="shared" ca="1" si="4"/>
-        <v>2.7576202181510405</v>
+        <v>3.9793506945470716</v>
       </c>
       <c r="E11" s="17">
         <f t="shared" ca="1" si="5"/>
-        <v>254.45244457594063</v>
+        <v>270.46555655885334</v>
       </c>
       <c r="F11" s="16">
         <f t="shared" ca="1" si="0"/>
@@ -1387,91 +2037,91 @@
       </c>
       <c r="G11" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>0.79582409652745523</v>
+        <v>0.97262306248562436</v>
       </c>
       <c r="H11" s="17">
         <f t="shared" ca="1" si="7"/>
-        <v>0.92036732051033798</v>
+        <v>1.3362637120549066</v>
       </c>
       <c r="I11" s="17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.60552787498698979</v>
+        <v>-0.23238842122852266</v>
       </c>
       <c r="J11" s="17">
         <f t="shared" ca="1" si="8"/>
-        <v>0.92036732051033809</v>
+        <v>1.8053289415348868</v>
       </c>
       <c r="K11" s="17">
         <f t="shared" ca="1" si="9"/>
-        <v>1.314265006453343</v>
+        <v>-4.1853335779117016</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
         <f t="shared" ca="1" si="2"/>
-        <v>114</v>
+        <v>252</v>
       </c>
       <c r="B12" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C12" s="17">
         <f t="shared" ca="1" si="10"/>
-        <v>2.689195104874246</v>
+        <v>0.29485645382257031</v>
       </c>
       <c r="D12" s="17">
         <f t="shared" ca="1" si="4"/>
-        <v>1.9896753472735358</v>
+        <v>4.3982297150257104</v>
       </c>
       <c r="E12" s="17">
         <f t="shared" ca="1" si="5"/>
-        <v>154.0795297965351</v>
+        <v>16.894030366227327</v>
       </c>
       <c r="F12" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G12" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>0.78498038868131048</v>
+        <v>0.623012211003653</v>
       </c>
       <c r="H12" s="17">
         <f t="shared" ca="1" si="7"/>
-        <v>0.90266447076744327</v>
+        <v>0.67258771281654095</v>
       </c>
       <c r="I12" s="17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.61952061255920987</v>
+        <v>0.78221210994227119</v>
       </c>
       <c r="J12" s="17">
         <f t="shared" ca="1" si="8"/>
-        <v>0.90266447076744338</v>
+        <v>0.67258771281654084</v>
       </c>
       <c r="K12" s="17">
         <f t="shared" ca="1" si="9"/>
-        <v>1.2670771121538542</v>
+        <v>0.79647477082607754</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A13" s="16">
         <f t="shared" ca="1" si="2"/>
-        <v>236</v>
+        <v>249</v>
       </c>
       <c r="B13" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13" s="17">
         <f t="shared" ca="1" si="10"/>
-        <v>5.5419819616041748</v>
+        <v>2.0090740878180742</v>
       </c>
       <c r="D13" s="17">
         <f t="shared" ca="1" si="4"/>
-        <v>4.1189770347066181</v>
+        <v>4.3458698374658802</v>
       </c>
       <c r="E13" s="17">
         <f t="shared" ca="1" si="5"/>
-        <v>317.53217653755229</v>
+        <v>115.11146596107137</v>
       </c>
       <c r="F13" s="16">
         <f t="shared" ca="1" si="0"/>
@@ -1479,75 +2129,75 @@
       </c>
       <c r="G13" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>-0.37143208943692263</v>
+        <v>-0.72716319344364899</v>
       </c>
       <c r="H13" s="17">
         <f t="shared" ca="1" si="7"/>
-        <v>-0.38055098076550709</v>
+        <v>-0.81418036640633418</v>
       </c>
       <c r="I13" s="17">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.92846012458076077</v>
+        <v>-0.68646463135461999</v>
       </c>
       <c r="J13" s="17">
         <f t="shared" ca="1" si="8"/>
-        <v>2.7610416728242857</v>
+        <v>2.327412287183459</v>
       </c>
       <c r="K13" s="17">
         <f t="shared" ca="1" si="9"/>
-        <v>0.40005174116081721</v>
+        <v>1.0592871944599935</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A14" s="16">
         <f t="shared" ca="1" si="2"/>
-        <v>342</v>
+        <v>1</v>
       </c>
       <c r="B14" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C14" s="17">
         <f t="shared" ca="1" si="10"/>
-        <v>1.3279110867861941</v>
+        <v>5.9722769844242016</v>
       </c>
       <c r="D14" s="17">
         <f t="shared" ca="1" si="4"/>
-        <v>5.9690260418206069</v>
+        <v>1.7453292519943295E-2</v>
       </c>
       <c r="E14" s="17">
         <f t="shared" ca="1" si="5"/>
-        <v>76.083700841479299</v>
+        <v>342.18626529062527</v>
       </c>
       <c r="F14" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G14" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>0.42013968223930687</v>
+        <v>0.8414709848078965</v>
       </c>
       <c r="H14" s="17">
         <f t="shared" ca="1" si="7"/>
-        <v>0.43359924128746302</v>
+        <v>1</v>
       </c>
       <c r="I14" s="17">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.907459446701534</v>
+        <v>0.54030230586813977</v>
       </c>
       <c r="J14" s="17">
         <f t="shared" ca="1" si="8"/>
-        <v>2.7079934123023301</v>
+        <v>0.99999999999999989</v>
       </c>
       <c r="K14" s="17">
         <f t="shared" ca="1" si="9"/>
-        <v>-0.46298452648925037</v>
+        <v>1.5574077246549023</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A15" s="16">
         <f t="shared" ca="1" si="2"/>
-        <v>140</v>
+        <v>303</v>
       </c>
       <c r="B15" s="16">
         <f t="shared" ca="1" si="3"/>
@@ -1555,315 +2205,315 @@
       </c>
       <c r="C15" s="17">
         <f t="shared" ca="1" si="10"/>
-        <v>5.2960755046610632</v>
+        <v>4.4834344232823202</v>
       </c>
       <c r="D15" s="17">
         <f t="shared" ca="1" si="4"/>
-        <v>2.4434609527920612</v>
+        <v>5.2883476335428181</v>
       </c>
       <c r="E15" s="17">
         <f t="shared" ca="1" si="5"/>
-        <v>303.44277439969648</v>
+        <v>256.8818701777472</v>
       </c>
       <c r="F15" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G15" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>0.98023965944031155</v>
+        <v>0.98663250484391052</v>
       </c>
       <c r="H15" s="17">
         <f t="shared" ca="1" si="7"/>
-        <v>1.371669411540696</v>
+        <v>1.4071052553798489</v>
       </c>
       <c r="I15" s="17">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.19781357400426822</v>
+        <v>0.16296103947088339</v>
       </c>
       <c r="J15" s="17">
         <f t="shared" ca="1" si="8"/>
-        <v>1.7699232420490976</v>
+        <v>1.4071052553798491</v>
       </c>
       <c r="K15" s="17">
         <f t="shared" ca="1" si="9"/>
-        <v>-4.9553710576967838</v>
+        <v>6.0544072868422907</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A16" s="16">
         <f t="shared" ca="1" si="2"/>
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="B16" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C16" s="17">
         <f t="shared" ca="1" si="10"/>
-        <v>6.7931759007375812</v>
+        <v>0.50080278308733761</v>
       </c>
       <c r="D16" s="17">
         <f t="shared" ca="1" si="4"/>
-        <v>4.5029494701453698</v>
+        <v>4.2935099599060509</v>
       </c>
       <c r="E16" s="17">
         <f t="shared" ca="1" si="5"/>
-        <v>389.22030860224487</v>
+        <v>28.693885839310088</v>
       </c>
       <c r="F16" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G16" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>0.37963562682930313</v>
+        <v>0.81675999962280854</v>
       </c>
       <c r="H16" s="17">
         <f t="shared" ca="1" si="7"/>
-        <v>0.38940240563695444</v>
+        <v>0.9557730199961274</v>
       </c>
       <c r="I16" s="17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.92513609314625822</v>
+        <v>0.5769775585030581</v>
       </c>
       <c r="J16" s="17">
         <f t="shared" ca="1" si="8"/>
-        <v>0.38940240563695427</v>
+        <v>0.9557730199961274</v>
       </c>
       <c r="K16" s="17">
         <f t="shared" ca="1" si="9"/>
-        <v>0.41035651904814957</v>
+        <v>1.4155836524073051</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A17" s="16">
         <f t="shared" ca="1" si="2"/>
-        <v>192</v>
+        <v>308</v>
       </c>
       <c r="B17" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17" s="17">
         <f t="shared" ca="1" si="10"/>
-        <v>8.0819249990407238E-2</v>
+        <v>6.7533808001965614</v>
       </c>
       <c r="D17" s="17">
         <f t="shared" ca="1" si="4"/>
-        <v>3.351032163829113</v>
+        <v>5.3756140961425354</v>
       </c>
       <c r="E17" s="17">
         <f t="shared" ca="1" si="5"/>
-        <v>4.6306019278630535</v>
+        <v>386.94021729594567</v>
       </c>
       <c r="F17" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G17" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>-0.35493835765184628</v>
+        <v>0.1236030360001129</v>
       </c>
       <c r="H17" s="17">
         <f t="shared" ca="1" si="7"/>
-        <v>-0.36284813102261243</v>
+        <v>0.12391994820026263</v>
       </c>
       <c r="I17" s="17">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.93488970593723519</v>
+        <v>0.99233174366819221</v>
       </c>
       <c r="J17" s="17">
         <f t="shared" ca="1" si="8"/>
-        <v>2.7787445225671807</v>
+        <v>0.12391994820026286</v>
       </c>
       <c r="K17" s="17">
         <f t="shared" ca="1" si="9"/>
-        <v>0.37965800179179154</v>
+        <v>0.12455818005298264</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A18" s="16">
         <f t="shared" ca="1" si="2"/>
-        <v>101</v>
+        <v>171</v>
       </c>
       <c r="B18" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C18" s="17">
         <f t="shared" ca="1" si="10"/>
-        <v>4.2102903144813624</v>
+        <v>0.88882407419963128</v>
       </c>
       <c r="D18" s="17">
         <f t="shared" ca="1" si="4"/>
-        <v>1.7627825445142729</v>
+        <v>2.9845130209103035</v>
       </c>
       <c r="E18" s="17">
         <f t="shared" ca="1" si="5"/>
-        <v>241.23186554459016</v>
+        <v>50.925868181261599</v>
       </c>
       <c r="F18" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>0.45202578717835057</v>
+        <v>0.97659086794356575</v>
       </c>
       <c r="H18" s="17">
         <f t="shared" ca="1" si="7"/>
-        <v>0.4690350851266164</v>
+        <v>1.3539967061511653</v>
       </c>
       <c r="I18" s="17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.89200486978816018</v>
+        <v>0.21510526876214117</v>
       </c>
       <c r="J18" s="17">
         <f t="shared" ca="1" si="8"/>
-        <v>0.46903508512661629</v>
+        <v>1.3539967061511651</v>
       </c>
       <c r="K18" s="17">
         <f t="shared" ca="1" si="9"/>
-        <v>0.50675260022481827</v>
+        <v>4.5400601926838862</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A19" s="16">
         <f t="shared" ca="1" si="2"/>
-        <v>232</v>
+        <v>12</v>
       </c>
       <c r="B19" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C19" s="17">
         <f t="shared" ca="1" si="10"/>
-        <v>0.23762813476282477</v>
+        <v>2.3468035785769974</v>
       </c>
       <c r="D19" s="17">
         <f t="shared" ca="1" si="4"/>
-        <v>4.0491638646268449</v>
+        <v>0.20943951023931956</v>
       </c>
       <c r="E19" s="17">
         <f t="shared" ca="1" si="5"/>
-        <v>13.615089215475821</v>
+        <v>134.4619403986602</v>
       </c>
       <c r="F19" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G19" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>-0.45987672323214268</v>
+        <v>-0.53657291800043494</v>
       </c>
       <c r="H19" s="17">
         <f t="shared" ca="1" si="7"/>
-        <v>-0.47785636564469963</v>
+        <v>-0.56637061435917291</v>
       </c>
       <c r="I19" s="17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.88798276978174939</v>
+        <v>0.84385395873249214</v>
       </c>
       <c r="J19" s="17">
         <f t="shared" ca="1" si="8"/>
-        <v>0.47785636564469947</v>
+        <v>0.56637061435917291</v>
       </c>
       <c r="K19" s="17">
         <f t="shared" ca="1" si="9"/>
-        <v>-0.51788924164054706</v>
+        <v>-0.63585992866158081</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A20" s="16">
         <f t="shared" ca="1" si="2"/>
-        <v>84</v>
+        <v>154</v>
       </c>
       <c r="B20" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C20" s="17">
         <f t="shared" ca="1" si="10"/>
-        <v>2.6712976036898235</v>
+        <v>5.3089784117959251</v>
       </c>
       <c r="D20" s="17">
         <f t="shared" ca="1" si="4"/>
-        <v>1.4660765716752369</v>
+        <v>2.6878070480712677</v>
       </c>
       <c r="E20" s="17">
         <f t="shared" ca="1" si="5"/>
-        <v>153.0540785148373</v>
+        <v>304.18205652197327</v>
       </c>
       <c r="F20" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>0.73319032007329221</v>
+        <v>-6.1920337256057306E-2</v>
       </c>
       <c r="H20" s="17">
         <f t="shared" ca="1" si="7"/>
-        <v>0.82300164692441746</v>
+        <v>-6.1959974100131314E-2</v>
       </c>
       <c r="I20" s="17">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.68002349558733877</v>
+        <v>-0.99808109481850027</v>
       </c>
       <c r="J20" s="17">
         <f t="shared" ca="1" si="8"/>
-        <v>2.3185910066653754</v>
+        <v>3.0796326794896602</v>
       </c>
       <c r="K20" s="17">
         <f t="shared" ca="1" si="9"/>
-        <v>-1.0781838051640156</v>
+        <v>6.2039384953301253E-2</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A21" s="16">
         <f t="shared" ca="1" si="2"/>
-        <v>272</v>
+        <v>108</v>
       </c>
       <c r="B21" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C21" s="17">
         <f t="shared" ca="1" si="10"/>
-        <v>0.64678022753624886</v>
+        <v>3.8887142861013277</v>
       </c>
       <c r="D21" s="17">
         <f t="shared" ca="1" si="4"/>
-        <v>4.7472955654245768</v>
+        <v>1.8849555921538759</v>
       </c>
       <c r="E21" s="17">
         <f t="shared" ca="1" si="5"/>
-        <v>37.057777310338132</v>
+        <v>222.806916325835</v>
       </c>
       <c r="F21" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G21" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>0.96835693843472415</v>
+        <v>0.92681850541778499</v>
       </c>
       <c r="H21" s="17">
         <f t="shared" ca="1" si="7"/>
-        <v>1.3185608623120117</v>
+        <v>1.1858497779470298</v>
       </c>
       <c r="I21" s="17">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.24956930858045798</v>
+        <v>0.37550959776701209</v>
       </c>
       <c r="J21" s="17">
         <f t="shared" ca="1" si="8"/>
-        <v>1.8230317912777814</v>
+        <v>1.1858497779470298</v>
       </c>
       <c r="K21" s="17">
         <f t="shared" ca="1" si="9"/>
-        <v>-3.8801122779988715</v>
+        <v>2.4681619615827688</v>
       </c>
     </row>
   </sheetData>
@@ -1907,351 +2557,351 @@
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="21">
         <f ca="1">$A$2 + RANDBETWEEN(1, NOW() - $A$2)</f>
-        <v>38331.03125</v>
+        <v>10217.03125</v>
       </c>
       <c r="B3" s="23">
         <f t="shared" ref="B3:B37" ca="1" si="0">A3</f>
-        <v>38331.03125</v>
+        <v>10217.03125</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="21">
         <f t="shared" ref="A4:A37" ca="1" si="1">$A$2 + RANDBETWEEN(1, NOW() - $A$2)</f>
-        <v>40616.03125</v>
+        <v>7565.03125</v>
       </c>
       <c r="B4" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>40616.03125</v>
+        <v>7565.03125</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>30294.03125</v>
+        <v>7515.03125</v>
       </c>
       <c r="B5" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>30294.03125</v>
+        <v>7515.03125</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>11995.03125</v>
+        <v>5702.03125</v>
       </c>
       <c r="B6" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>11995.03125</v>
+        <v>5702.03125</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>26167.03125</v>
+        <v>26857.03125</v>
       </c>
       <c r="B7" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>26167.03125</v>
+        <v>26857.03125</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>31258.03125</v>
+        <v>38559.03125</v>
       </c>
       <c r="B8" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>31258.03125</v>
+        <v>38559.03125</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>9328.03125</v>
+        <v>9000.03125</v>
       </c>
       <c r="B9" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>9328.03125</v>
+        <v>9000.03125</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>10249.03125</v>
+        <v>38095.03125</v>
       </c>
       <c r="B10" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>10249.03125</v>
+        <v>38095.03125</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>10568.03125</v>
+        <v>18707.03125</v>
       </c>
       <c r="B11" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>10568.03125</v>
+        <v>18707.03125</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>2424.03125</v>
+        <v>29479.03125</v>
       </c>
       <c r="B12" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>2424.03125</v>
+        <v>29479.03125</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>639.03125</v>
+        <v>10969.03125</v>
       </c>
       <c r="B13" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>639.03125</v>
+        <v>10969.03125</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>38636.03125</v>
+        <v>30777.03125</v>
       </c>
       <c r="B14" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>38636.03125</v>
+        <v>30777.03125</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>1186.03125</v>
+        <v>26237.03125</v>
       </c>
       <c r="B15" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>1186.03125</v>
+        <v>26237.03125</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>7724.03125</v>
+        <v>17493.03125</v>
       </c>
       <c r="B16" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>7724.03125</v>
+        <v>17493.03125</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>41246.03125</v>
+        <v>16500.03125</v>
       </c>
       <c r="B17" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>41246.03125</v>
+        <v>16500.03125</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>19048.03125</v>
+        <v>32798.03125</v>
       </c>
       <c r="B18" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>19048.03125</v>
+        <v>32798.03125</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>23838.03125</v>
+        <v>36180.03125</v>
       </c>
       <c r="B19" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>23838.03125</v>
+        <v>36180.03125</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>26225.03125</v>
+        <v>16224.03125</v>
       </c>
       <c r="B20" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>26225.03125</v>
+        <v>16224.03125</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>13997.03125</v>
+        <v>5272.03125</v>
       </c>
       <c r="B21" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>13997.03125</v>
+        <v>5272.03125</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>34037.03125</v>
+        <v>40653.03125</v>
       </c>
       <c r="B22" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>34037.03125</v>
+        <v>40653.03125</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>32596.03125</v>
+        <v>32552.03125</v>
       </c>
       <c r="B23" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>32596.03125</v>
+        <v>32552.03125</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>33108.03125</v>
+        <v>13790.03125</v>
       </c>
       <c r="B24" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>33108.03125</v>
+        <v>13790.03125</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>36165.03125</v>
+        <v>20322.03125</v>
       </c>
       <c r="B25" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>36165.03125</v>
+        <v>20322.03125</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>2159.03125</v>
+        <v>35074.03125</v>
       </c>
       <c r="B26" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>2159.03125</v>
+        <v>35074.03125</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>4623.03125</v>
+        <v>35351.03125</v>
       </c>
       <c r="B27" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>4623.03125</v>
+        <v>35351.03125</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>36095.03125</v>
+        <v>6013.03125</v>
       </c>
       <c r="B28" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>36095.03125</v>
+        <v>6013.03125</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>28543.03125</v>
+        <v>25527.03125</v>
       </c>
       <c r="B29" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>28543.03125</v>
+        <v>25527.03125</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>20410.03125</v>
+        <v>23061.03125</v>
       </c>
       <c r="B30" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>20410.03125</v>
+        <v>23061.03125</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>13303.03125</v>
+        <v>33856.03125</v>
       </c>
       <c r="B31" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>13303.03125</v>
+        <v>33856.03125</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>16538.03125</v>
+        <v>35999.03125</v>
       </c>
       <c r="B32" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>16538.03125</v>
+        <v>35999.03125</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>29784.03125</v>
+        <v>27793.03125</v>
       </c>
       <c r="B33" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>29784.03125</v>
+        <v>27793.03125</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>6229.03125</v>
+        <v>35621.03125</v>
       </c>
       <c r="B34" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>6229.03125</v>
+        <v>35621.03125</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>12157.03125</v>
+        <v>39696.03125</v>
       </c>
       <c r="B35" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>12157.03125</v>
+        <v>39696.03125</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>14583.03125</v>
+        <v>40518.03125</v>
       </c>
       <c r="B36" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>14583.03125</v>
+        <v>40518.03125</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>8759.03125</v>
+        <v>15171.03125</v>
       </c>
       <c r="B37" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>8759.03125</v>
+        <v>15171.03125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactored tests. Refactored SolarTimes. Added TrueSolarTime. Added Excel Mod function.
git-svn-id: https://solarcalculator.svn.codeplex.com/svn@26906 937343c3-697a-4e39-b5c6-83b50a1b7d63
</commit_message>
<xml_diff>
--- a/Source/Innovative.SolarCalculator.Tests/NOAA Solar Calculations Test Data.xlsx
+++ b/Source/Innovative.SolarCalculator.Tests/NOAA Solar Calculations Test Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="339"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="339" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Calculations" sheetId="1" r:id="rId1"/>
@@ -613,7 +613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -5834,18 +5834,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" style="19" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" style="19" customWidth="1"/>
+    <col min="1" max="2" width="29" style="20" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.7109375" style="19" customWidth="1"/>
     <col min="4" max="4" width="30.28515625" style="20" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29" style="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="19" customWidth="1"/>
+    <col min="6" max="6" width="29" style="20" bestFit="1" customWidth="1"/>
     <col min="7" max="9" width="31.5703125" style="20" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="30.28515625" style="20" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="31.5703125" style="20" customWidth="1"/>
@@ -5853,10 +5852,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="17" t="s">
         <v>42</v>
       </c>
       <c r="C1" s="16" t="s">
@@ -5868,7 +5867,7 @@
       <c r="E1" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="17" t="s">
         <v>35</v>
       </c>
       <c r="G1" s="17" t="s">
@@ -5888,923 +5887,923 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="16">
-        <f ca="1">RANDBETWEEN(1,360)</f>
-        <v>204</v>
-      </c>
-      <c r="B2" s="16">
-        <f ca="1">RANDBETWEEN(1,5)</f>
-        <v>2</v>
+      <c r="A2" s="17">
+        <f ca="1">RANDBETWEEN(1,360) + (RANDBETWEEN(0,10000000000000000000)/10000000000000000000)</f>
+        <v>115.5315107116607</v>
+      </c>
+      <c r="B2" s="17">
+        <f ca="1">RANDBETWEEN(1,360) + (RANDBETWEEN(0,10000000000000000000)/10000000000000000000)</f>
+        <v>124.09841474777483</v>
       </c>
       <c r="C2" s="17">
         <f ca="1">RANDBETWEEN(0,2*PI()) + (RANDBETWEEN(0,10000000000000000000)/10000000000000000000)</f>
-        <v>4.8216990477245609</v>
+        <v>6.9579848565336144</v>
       </c>
       <c r="D2" s="17">
         <f ca="1">RADIANS(A2)</f>
-        <v>3.5604716740684323</v>
+        <v>2.0164052517215763</v>
       </c>
       <c r="E2" s="17">
         <f ca="1">DEGREES(C2)</f>
-        <v>276.26300551686546</v>
-      </c>
-      <c r="F2" s="16">
+        <v>398.66316619531574</v>
+      </c>
+      <c r="F2" s="17">
         <f t="shared" ref="F2:F21" ca="1" si="0">MOD(A2,B2)</f>
-        <v>0</v>
+        <v>115.5315107116607</v>
       </c>
       <c r="G2" s="17">
         <f ca="1">SIN(A2)</f>
-        <v>0.20212035931279121</v>
+        <v>0.64987310809703713</v>
       </c>
       <c r="H2" s="17">
         <f ca="1">ASIN(G2)</f>
-        <v>0.20352248333656048</v>
+        <v>0.70741747116164888</v>
       </c>
       <c r="I2" s="17">
         <f t="shared" ref="I2:I21" ca="1" si="1">COS(A2)</f>
-        <v>-0.97936068960892453</v>
+        <v>-0.76004272470190559</v>
       </c>
       <c r="J2" s="17">
         <f ca="1">ACOS(I2)</f>
-        <v>2.9380701702532326</v>
+        <v>2.4341751824281443</v>
       </c>
       <c r="K2" s="17">
         <f ca="1">TAN(A2)</f>
-        <v>-0.20637989808790605</v>
+        <v>-0.85504812686934439</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="16">
-        <f t="shared" ref="A3:A21" ca="1" si="2">RANDBETWEEN(1,360)</f>
-        <v>267</v>
-      </c>
-      <c r="B3" s="16">
-        <f t="shared" ref="B3:B21" ca="1" si="3">RANDBETWEEN(1,5)</f>
-        <v>2</v>
+      <c r="A3" s="17">
+        <f t="shared" ref="A3:A21" ca="1" si="2">RANDBETWEEN(1,360) + (RANDBETWEEN(0,10000000000000000000)/10000000000000000000)</f>
+        <v>322.95898197512804</v>
+      </c>
+      <c r="B3" s="17">
+        <f t="shared" ref="B3:B21" ca="1" si="3">RANDBETWEEN(1,360) + (RANDBETWEEN(0,10000000000000000000)/10000000000000000000)</f>
+        <v>128.39932782873524</v>
       </c>
       <c r="C3" s="17">
         <f ca="1">RANDBETWEEN(0,2*PI()) + (RANDBETWEEN(0,10000000000000000000)/10000000000000000000)</f>
-        <v>4.2777598217726842</v>
+        <v>6.5697452105302636</v>
       </c>
       <c r="D3" s="17">
         <f t="shared" ref="D3:D21" ca="1" si="4">RADIANS(A3)</f>
-        <v>4.6600291028248595</v>
+        <v>5.6366975843550042</v>
       </c>
       <c r="E3" s="17">
         <f t="shared" ref="E3:E21" ca="1" si="5">DEGREES(C3)</f>
-        <v>245.09758355821006</v>
-      </c>
-      <c r="F3" s="16">
+        <v>376.41867303967058</v>
+      </c>
+      <c r="F3" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>66.160326317657564</v>
       </c>
       <c r="G3" s="17">
         <f t="shared" ref="G3:G21" ca="1" si="6">SIN(A3)</f>
-        <v>3.5368177256176046E-2</v>
+        <v>0.58514702006446095</v>
       </c>
       <c r="H3" s="17">
         <f t="shared" ref="H3:H21" ca="1" si="7">ASIN(G3)</f>
-        <v>3.5375555132425275E-2</v>
+        <v>0.62506134462066343</v>
       </c>
       <c r="I3" s="17">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.99937435030001431</v>
+        <v>-0.81092722540908768</v>
       </c>
       <c r="J3" s="17">
         <f t="shared" ref="J3:J21" ca="1" si="8">ACOS(I3)</f>
-        <v>3.106217098457368</v>
+        <v>2.5165313089691299</v>
       </c>
       <c r="K3" s="17">
         <f t="shared" ref="K3:K21" ca="1" si="9">TAN(A3)</f>
-        <v>-3.5390319198765154E-2</v>
+        <v>-0.721577722056714</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="16">
+      <c r="A4" s="17">
         <f t="shared" ca="1" si="2"/>
-        <v>203</v>
-      </c>
-      <c r="B4" s="16">
+        <v>18.356125395144488</v>
+      </c>
+      <c r="B4" s="17">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>269.22494908715959</v>
       </c>
       <c r="C4" s="17">
         <f t="shared" ref="C4:C21" ca="1" si="10">RANDBETWEEN(0,2*PI()) + (RANDBETWEEN(0,10000000000000000000)/10000000000000000000)</f>
-        <v>0.74314438820493445</v>
+        <v>0.85044854606701292</v>
       </c>
       <c r="D4" s="17">
         <f t="shared" ca="1" si="4"/>
-        <v>3.5430183815484888</v>
+        <v>0.32037482605421647</v>
       </c>
       <c r="E4" s="17">
         <f t="shared" ca="1" si="5"/>
-        <v>42.579037012974382</v>
-      </c>
-      <c r="F4" s="16">
+        <v>48.727112382677007</v>
+      </c>
+      <c r="F4" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>18.356125395144488</v>
       </c>
       <c r="G4" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>0.93330970016696035</v>
+        <v>-0.47364997911386936</v>
       </c>
       <c r="H4" s="17">
         <f t="shared" ca="1" si="7"/>
-        <v>1.2035224833365603</v>
+        <v>-0.49343052639427121</v>
       </c>
       <c r="I4" s="17">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.35907242107165305</v>
+        <v>0.88071317537858551</v>
       </c>
       <c r="J4" s="17">
         <f t="shared" ca="1" si="8"/>
-        <v>1.9380701702532326</v>
+        <v>0.4934305263942711</v>
       </c>
       <c r="K4" s="17">
         <f t="shared" ca="1" si="9"/>
-        <v>-2.5992241269365493</v>
+        <v>-0.53780276298269869</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="16">
+      <c r="A5" s="17">
         <f t="shared" ca="1" si="2"/>
-        <v>339</v>
-      </c>
-      <c r="B5" s="16">
+        <v>188.97968062583112</v>
+      </c>
+      <c r="B5" s="17">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>73.211205179287461</v>
       </c>
       <c r="C5" s="17">
         <f t="shared" ca="1" si="10"/>
-        <v>2.6887766275036662</v>
+        <v>1.9752403624847394</v>
       </c>
       <c r="D5" s="17">
         <f t="shared" ca="1" si="4"/>
-        <v>5.9166661642607767</v>
+        <v>3.2983176462880914</v>
       </c>
       <c r="E5" s="17">
         <f t="shared" ca="1" si="5"/>
-        <v>154.05555280937915</v>
-      </c>
-      <c r="F5" s="16">
+        <v>113.17293629426644</v>
+      </c>
+      <c r="F5" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>42.5572702672562</v>
       </c>
       <c r="G5" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>-0.28787444850848609</v>
+        <v>0.46543091343983561</v>
       </c>
       <c r="H5" s="17">
         <f t="shared" ca="1" si="7"/>
-        <v>-0.29200658769766979</v>
+        <v>0.48412141044352774</v>
       </c>
       <c r="I5" s="17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.95766815854759157</v>
+        <v>0.88508421340263443</v>
       </c>
       <c r="J5" s="17">
         <f t="shared" ca="1" si="8"/>
-        <v>0.29200658769766963</v>
+        <v>0.48412141044352786</v>
       </c>
       <c r="K5" s="17">
         <f t="shared" ca="1" si="9"/>
-        <v>-0.30059937352942706</v>
+        <v>0.52586059766055959</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="16">
+      <c r="A6" s="17">
         <f t="shared" ca="1" si="2"/>
-        <v>159</v>
-      </c>
-      <c r="B6" s="16">
+        <v>8.2420355875180658</v>
+      </c>
+      <c r="B6" s="17">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>57.597087578377426</v>
       </c>
       <c r="C6" s="17">
         <f t="shared" ca="1" si="10"/>
-        <v>0.92419324282303117</v>
+        <v>6.9092476171140085</v>
       </c>
       <c r="D6" s="17">
         <f t="shared" ca="1" si="4"/>
-        <v>2.7750735106709841</v>
+        <v>0.14385065806873551</v>
       </c>
       <c r="E6" s="17">
         <f t="shared" ca="1" si="5"/>
-        <v>52.952372268268945</v>
-      </c>
-      <c r="F6" s="16">
+        <v>395.87072807145364</v>
+      </c>
+      <c r="F6" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>8.2420355875180658</v>
       </c>
       <c r="G6" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>0.93951973171314829</v>
+        <v>0.92564717234882221</v>
       </c>
       <c r="H6" s="17">
         <f t="shared" ca="1" si="7"/>
-        <v>1.2212253330794554</v>
+        <v>1.1827423732513138</v>
       </c>
       <c r="I6" s="17">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.34249477911590703</v>
+        <v>-0.37838778035585363</v>
       </c>
       <c r="J6" s="17">
         <f t="shared" ca="1" si="8"/>
-        <v>1.920367320510338</v>
+        <v>1.9588502803384793</v>
       </c>
       <c r="K6" s="17">
         <f t="shared" ca="1" si="9"/>
-        <v>-2.7431651195920748</v>
+        <v>-2.4462924555288232</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="16">
+      <c r="A7" s="17">
         <f t="shared" ca="1" si="2"/>
-        <v>341</v>
-      </c>
-      <c r="B7" s="16">
+        <v>186.25427466717872</v>
+      </c>
+      <c r="B7" s="17">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>56.420850807654581</v>
       </c>
       <c r="C7" s="17">
         <f t="shared" ca="1" si="10"/>
-        <v>2.0149919306654414</v>
+        <v>2.5689646828089217</v>
       </c>
       <c r="D7" s="17">
         <f t="shared" ca="1" si="4"/>
-        <v>5.9515727493006638</v>
+        <v>3.2507503388561343</v>
       </c>
       <c r="E7" s="17">
         <f t="shared" ca="1" si="5"/>
-        <v>115.45053338004719</v>
-      </c>
-      <c r="F7" s="16">
+        <v>147.19083404311544</v>
+      </c>
+      <c r="F7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>16.991722244214976</v>
       </c>
       <c r="G7" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>0.99060323338977374</v>
+        <v>-0.78351839382031951</v>
       </c>
       <c r="H7" s="17">
         <f t="shared" ca="1" si="7"/>
-        <v>1.4335992412874632</v>
+        <v>-0.90030810538091866</v>
       </c>
       <c r="I7" s="17">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.13676707936387883</v>
+        <v>-0.62136859153422508</v>
       </c>
       <c r="J7" s="17">
         <f t="shared" ca="1" si="8"/>
-        <v>1.7079934123023301</v>
+        <v>2.2412845482088741</v>
       </c>
       <c r="K7" s="17">
         <f t="shared" ca="1" si="9"/>
-        <v>-7.242994717714204</v>
+        <v>1.2609559036219216</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="16">
+      <c r="A8" s="17">
         <f t="shared" ca="1" si="2"/>
-        <v>356</v>
-      </c>
-      <c r="B8" s="16">
+        <v>256.01604234941834</v>
+      </c>
+      <c r="B8" s="17">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>176.99605234925255</v>
       </c>
       <c r="C8" s="17">
         <f t="shared" ca="1" si="10"/>
-        <v>4.3712100452407121</v>
+        <v>4.3878470914161616</v>
       </c>
       <c r="D8" s="17">
         <f t="shared" ca="1" si="4"/>
-        <v>6.213372137099813</v>
+        <v>4.4683228769225893</v>
       </c>
       <c r="E8" s="17">
         <f t="shared" ca="1" si="5"/>
-        <v>250.45188695748246</v>
-      </c>
-      <c r="F8" s="16">
+        <v>251.40511948689996</v>
+      </c>
+      <c r="F8" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>79.019990000165791</v>
       </c>
       <c r="G8" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>-0.84148727148921076</v>
+        <v>-0.99971777018078645</v>
       </c>
       <c r="H8" s="17">
         <f t="shared" ca="1" si="7"/>
-        <v>-1.0000301443533641</v>
+        <v>-1.5470374086450907</v>
       </c>
       <c r="I8" s="17">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.54027694002395044</v>
+        <v>-2.3756682949357583E-2</v>
       </c>
       <c r="J8" s="17">
         <f t="shared" ca="1" si="8"/>
-        <v>2.141562509236429</v>
+        <v>1.5945552449447036</v>
       </c>
       <c r="K8" s="17">
         <f t="shared" ca="1" si="9"/>
-        <v>1.5575109895527055</v>
+        <v>42.081538584822518</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="16">
+      <c r="A9" s="17">
         <f t="shared" ca="1" si="2"/>
-        <v>338</v>
-      </c>
-      <c r="B9" s="16">
+        <v>79.327886296596176</v>
+      </c>
+      <c r="B9" s="17">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>229.42069243045535</v>
       </c>
       <c r="C9" s="17">
         <f t="shared" ca="1" si="10"/>
-        <v>5.8389362183818188</v>
+        <v>4.6768952244997637</v>
       </c>
       <c r="D9" s="17">
         <f t="shared" ca="1" si="4"/>
-        <v>5.8992128717408336</v>
+        <v>1.3845328045232943</v>
       </c>
       <c r="E9" s="17">
         <f t="shared" ca="1" si="5"/>
-        <v>334.54640215935541</v>
-      </c>
-      <c r="F9" s="16">
+        <v>267.96635758872611</v>
+      </c>
+      <c r="F9" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>79.327886296596176</v>
       </c>
       <c r="G9" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>-0.96138919682186075</v>
+        <v>-0.70899349837560954</v>
       </c>
       <c r="H9" s="17">
         <f t="shared" ca="1" si="7"/>
-        <v>-1.2920065876976694</v>
+        <v>-0.78806995685134551</v>
       </c>
       <c r="I9" s="17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.27519231863229304</v>
+        <v>-0.70521501633268879</v>
       </c>
       <c r="J9" s="17">
         <f t="shared" ca="1" si="8"/>
-        <v>1.2920065876976696</v>
+        <v>2.3535226967384477</v>
       </c>
       <c r="K9" s="17">
         <f t="shared" ca="1" si="9"/>
-        <v>-3.4935175574666069</v>
+        <v>1.0053579148988769</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="16">
+      <c r="A10" s="17">
         <f t="shared" ca="1" si="2"/>
-        <v>137</v>
-      </c>
-      <c r="B10" s="16">
+        <v>17.984877278315068</v>
+      </c>
+      <c r="B10" s="17">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>217.35200374294152</v>
       </c>
       <c r="C10" s="17">
         <f t="shared" ca="1" si="10"/>
-        <v>6.7120411667293798</v>
+        <v>1.3247088958217055</v>
       </c>
       <c r="D10" s="17">
         <f t="shared" ca="1" si="4"/>
-        <v>2.3911010752322315</v>
+        <v>0.31389532407371451</v>
       </c>
       <c r="E10" s="17">
         <f t="shared" ca="1" si="5"/>
-        <v>384.57163077165836</v>
-      </c>
-      <c r="F10" s="16">
+        <v>75.900228814019172</v>
+      </c>
+      <c r="F10" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>17.984877278315068</v>
       </c>
       <c r="G10" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>-0.94251445455825089</v>
+        <v>-0.76088677943917138</v>
       </c>
       <c r="H10" s="17">
         <f t="shared" ca="1" si="7"/>
-        <v>-1.2300767579509024</v>
+        <v>-0.86467864322369159</v>
       </c>
       <c r="I10" s="17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.33416538263076073</v>
+        <v>0.64888466531016575</v>
       </c>
       <c r="J10" s="17">
         <f t="shared" ca="1" si="8"/>
-        <v>1.2300767579509024</v>
+        <v>0.86467864322369148</v>
       </c>
       <c r="K10" s="17">
         <f t="shared" ca="1" si="9"/>
-        <v>-2.8205029711281955</v>
+        <v>-1.1726071212909135</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="16">
+      <c r="A11" s="17">
         <f t="shared" ca="1" si="2"/>
-        <v>218</v>
-      </c>
-      <c r="B11" s="16">
+        <v>17.364654166514736</v>
+      </c>
+      <c r="B11" s="17">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>138.46272200847591</v>
       </c>
       <c r="C11" s="17">
         <f t="shared" ca="1" si="10"/>
-        <v>6.6181939265725305</v>
+        <v>5.0901829002549341</v>
       </c>
       <c r="D11" s="17">
         <f t="shared" ca="1" si="4"/>
-        <v>3.8048177693476384</v>
+        <v>0.3030703886758338</v>
       </c>
       <c r="E11" s="17">
         <f t="shared" ca="1" si="5"/>
-        <v>379.19457999172027</v>
-      </c>
-      <c r="F11" s="16">
+        <v>291.64599713426861</v>
+      </c>
+      <c r="F11" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>17.364654166514736</v>
       </c>
       <c r="G11" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>-0.94252452732940251</v>
+        <v>-0.99631332875726952</v>
       </c>
       <c r="H11" s="17">
         <f t="shared" ca="1" si="7"/>
-        <v>-1.2301069023042666</v>
+        <v>-1.4849017550240249</v>
       </c>
       <c r="I11" s="17">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.33413697099017109</v>
+        <v>8.5788990789080907E-2</v>
       </c>
       <c r="J11" s="17">
         <f t="shared" ca="1" si="8"/>
-        <v>1.9114857512855268</v>
+        <v>1.4849017550240233</v>
       </c>
       <c r="K11" s="17">
         <f t="shared" ca="1" si="9"/>
-        <v>2.82077294391086</v>
+        <v>-11.613533620028068</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="16">
+      <c r="A12" s="17">
         <f t="shared" ca="1" si="2"/>
-        <v>309</v>
-      </c>
-      <c r="B12" s="16">
+        <v>258.18235093630562</v>
+      </c>
+      <c r="B12" s="17">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>1.686276807999405</v>
       </c>
       <c r="C12" s="17">
         <f t="shared" ca="1" si="10"/>
-        <v>3.2629385299275757</v>
+        <v>5.1059319797574778</v>
       </c>
       <c r="D12" s="17">
         <f t="shared" ca="1" si="4"/>
-        <v>5.3930673886624785</v>
+        <v>4.5061320943779979</v>
       </c>
       <c r="E12" s="17">
         <f t="shared" ca="1" si="5"/>
-        <v>186.95260657547135</v>
-      </c>
-      <c r="F12" s="16">
+        <v>292.54835292098034</v>
+      </c>
+      <c r="F12" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>0.18199931239665235</v>
       </c>
       <c r="G12" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>0.90180137496377455</v>
+        <v>0.54110735879853311</v>
       </c>
       <c r="H12" s="17">
         <f t="shared" ca="1" si="7"/>
-        <v>1.1239199482002626</v>
+        <v>0.57175334194257899</v>
       </c>
       <c r="I12" s="17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.43215076086181514</v>
+        <v>0.84095352205343399</v>
       </c>
       <c r="J12" s="17">
         <f t="shared" ca="1" si="8"/>
-        <v>1.1239199482002626</v>
+        <v>0.5717533419425791</v>
       </c>
       <c r="K12" s="17">
         <f t="shared" ca="1" si="9"/>
-        <v>2.0867749328159468</v>
+        <v>0.64344502354572608</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="16">
+      <c r="A13" s="17">
         <f t="shared" ca="1" si="2"/>
-        <v>172</v>
-      </c>
-      <c r="B13" s="16">
+        <v>343.79798153728711</v>
+      </c>
+      <c r="B13" s="17">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>198.53811812687312</v>
       </c>
       <c r="C13" s="17">
         <f t="shared" ca="1" si="10"/>
-        <v>2.7962034135639802E-2</v>
+        <v>4.9750745627650961</v>
       </c>
       <c r="D13" s="17">
         <f t="shared" ca="1" si="4"/>
-        <v>3.001966313430247</v>
+        <v>6.0004067395363361</v>
       </c>
       <c r="E13" s="17">
         <f t="shared" ca="1" si="5"/>
-        <v>1.6021065425728995</v>
-      </c>
-      <c r="F13" s="16">
+        <v>285.05077520933338</v>
+      </c>
+      <c r="F13" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>145.259863410414</v>
       </c>
       <c r="G13" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>0.70865914018232268</v>
+        <v>-0.97877215557464625</v>
       </c>
       <c r="H13" s="17">
         <f t="shared" ca="1" si="7"/>
-        <v>0.78759594743862815</v>
+        <v>-1.3643822959996517</v>
       </c>
       <c r="I13" s="17">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.70555100668629989</v>
+        <v>-0.2049513783114438</v>
       </c>
       <c r="J13" s="17">
         <f t="shared" ca="1" si="8"/>
-        <v>2.3539967061511651</v>
+        <v>1.7772103575901417</v>
       </c>
       <c r="K13" s="17">
         <f t="shared" ca="1" si="9"/>
-        <v>-1.0044052569786848</v>
+        <v>4.7756309991109474</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="16">
+      <c r="A14" s="17">
         <f t="shared" ca="1" si="2"/>
-        <v>243</v>
-      </c>
-      <c r="B14" s="16">
+        <v>233.28228016359878</v>
+      </c>
+      <c r="B14" s="17">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>152.93276653387736</v>
       </c>
       <c r="C14" s="17">
         <f t="shared" ca="1" si="10"/>
-        <v>2.072538851164559</v>
+        <v>4.8521232708603916</v>
       </c>
       <c r="D14" s="17">
         <f t="shared" ca="1" si="4"/>
-        <v>4.2411500823462207</v>
+        <v>4.0715438754146547</v>
       </c>
       <c r="E14" s="17">
         <f t="shared" ca="1" si="5"/>
-        <v>118.74772904862152</v>
-      </c>
-      <c r="F14" s="16">
+        <v>278.0061850975128</v>
+      </c>
+      <c r="F14" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>80.349513629721429</v>
       </c>
       <c r="G14" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>-0.89000934885627714</v>
+        <v>0.72043115124847701</v>
       </c>
       <c r="H14" s="17">
         <f t="shared" ca="1" si="7"/>
-        <v>-1.0973656735859207</v>
+        <v>0.80442379795408481</v>
       </c>
       <c r="I14" s="17">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.4559422758951242</v>
+        <v>0.69352646403060503</v>
       </c>
       <c r="J14" s="17">
         <f t="shared" ca="1" si="8"/>
-        <v>2.0442269800038724</v>
+        <v>0.80442379795408459</v>
       </c>
       <c r="K14" s="17">
         <f t="shared" ca="1" si="9"/>
-        <v>1.9520219903034328</v>
+        <v>1.0387940311051846</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="16">
+      <c r="A15" s="17">
         <f t="shared" ca="1" si="2"/>
-        <v>147</v>
-      </c>
-      <c r="B15" s="16">
+        <v>241.64956082772829</v>
+      </c>
+      <c r="B15" s="17">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>263.91367599149157</v>
       </c>
       <c r="C15" s="17">
         <f t="shared" ca="1" si="10"/>
-        <v>6.6437940909591111</v>
+        <v>2.1472064442878644</v>
       </c>
       <c r="D15" s="17">
         <f t="shared" ca="1" si="4"/>
-        <v>2.5656340004316642</v>
+        <v>4.2175804724421724</v>
       </c>
       <c r="E15" s="17">
         <f t="shared" ca="1" si="5"/>
-        <v>380.66136136591246</v>
-      </c>
-      <c r="F15" s="16">
+        <v>123.02586700098696</v>
+      </c>
+      <c r="F15" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>241.64956082772829</v>
       </c>
       <c r="G15" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>0.60904402188329243</v>
+        <v>0.25038073708407116</v>
       </c>
       <c r="H15" s="17">
         <f t="shared" ca="1" si="7"/>
-        <v>0.65485471872028223</v>
+        <v>0.25307349868578533</v>
       </c>
       <c r="I15" s="17">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.79313641916647837</v>
+        <v>-0.96814745080345965</v>
       </c>
       <c r="J15" s="17">
         <f t="shared" ca="1" si="8"/>
-        <v>2.4867379348695113</v>
+        <v>2.8885191549040075</v>
       </c>
       <c r="K15" s="17">
         <f t="shared" ca="1" si="9"/>
-        <v>-0.76789314822202714</v>
+        <v>-0.25861839214293414</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="16">
+      <c r="A16" s="17">
         <f t="shared" ca="1" si="2"/>
-        <v>68</v>
-      </c>
-      <c r="B16" s="16">
+        <v>298.90133809111916</v>
+      </c>
+      <c r="B16" s="17">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>168.99739411310603</v>
       </c>
       <c r="C16" s="17">
         <f t="shared" ca="1" si="10"/>
-        <v>4.6067587872305813</v>
+        <v>4.2307560411862264</v>
       </c>
       <c r="D16" s="17">
         <f t="shared" ca="1" si="4"/>
-        <v>1.1868238913561442</v>
+        <v>5.2168124883067719</v>
       </c>
       <c r="E16" s="17">
         <f t="shared" ca="1" si="5"/>
-        <v>263.94783574311793</v>
-      </c>
-      <c r="F16" s="16">
+        <v>242.40446530944706</v>
+      </c>
+      <c r="F16" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>129.90394397801313</v>
       </c>
       <c r="G16" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>-0.8979276806892913</v>
+        <v>-0.4349979500050084</v>
       </c>
       <c r="H16" s="17">
         <f t="shared" ca="1" si="7"/>
-        <v>-1.1150383789754514</v>
+        <v>-0.45003600008879985</v>
       </c>
       <c r="I16" s="17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.4401430224960407</v>
+        <v>-0.90043144297133482</v>
       </c>
       <c r="J16" s="17">
         <f t="shared" ca="1" si="8"/>
-        <v>1.1150383789754512</v>
+        <v>2.6915566535009936</v>
       </c>
       <c r="K16" s="17">
         <f t="shared" ca="1" si="9"/>
-        <v>-2.0400815980159464</v>
+        <v>0.48309946681732724</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="16">
+      <c r="A17" s="17">
         <f t="shared" ca="1" si="2"/>
-        <v>68</v>
-      </c>
-      <c r="B17" s="16">
+        <v>105.09225525014067</v>
+      </c>
+      <c r="B17" s="17">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>325.55814772664075</v>
       </c>
       <c r="C17" s="17">
         <f t="shared" ca="1" si="10"/>
-        <v>2.1117440467791972</v>
+        <v>6.949772294902445</v>
       </c>
       <c r="D17" s="17">
         <f t="shared" ca="1" si="4"/>
-        <v>1.1868238913561442</v>
+        <v>1.8342058724612516</v>
       </c>
       <c r="E17" s="17">
         <f t="shared" ca="1" si="5"/>
-        <v>120.99402129232509</v>
-      </c>
-      <c r="F17" s="16">
+        <v>398.19262107485861</v>
+      </c>
+      <c r="F17" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>105.09225525014067</v>
       </c>
       <c r="G17" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>-0.8979276806892913</v>
+        <v>-0.98860630176075981</v>
       </c>
       <c r="H17" s="17">
         <f t="shared" ca="1" si="7"/>
-        <v>-1.1150383789754514</v>
+        <v>-1.4196976816774904</v>
       </c>
       <c r="I17" s="17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.4401430224960407</v>
+        <v>-0.15052435058459349</v>
       </c>
       <c r="J17" s="17">
         <f t="shared" ca="1" si="8"/>
-        <v>1.1150383789754512</v>
+        <v>1.7218949719123029</v>
       </c>
       <c r="K17" s="17">
         <f t="shared" ca="1" si="9"/>
-        <v>-2.0400815980159464</v>
+        <v>6.5677499881002364</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="16">
+      <c r="A18" s="17">
         <f t="shared" ca="1" si="2"/>
-        <v>228</v>
-      </c>
-      <c r="B18" s="16">
+        <v>214.94730367819218</v>
+      </c>
+      <c r="B18" s="17">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>351.05887297370276</v>
       </c>
       <c r="C18" s="17">
         <f t="shared" ca="1" si="10"/>
-        <v>4.0859250630532022</v>
+        <v>3.8865649346976365</v>
       </c>
       <c r="D18" s="17">
         <f t="shared" ca="1" si="4"/>
-        <v>3.9793506945470716</v>
+        <v>3.7515381674685715</v>
       </c>
       <c r="E18" s="17">
         <f t="shared" ca="1" si="5"/>
-        <v>234.10626151967327</v>
-      </c>
-      <c r="F18" s="16">
+        <v>222.68376756171298</v>
+      </c>
+      <c r="F18" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>214.94730367819218</v>
       </c>
       <c r="G18" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>0.97262306248562436</v>
+        <v>0.96846724609872181</v>
       </c>
       <c r="H18" s="17">
         <f t="shared" ca="1" si="7"/>
-        <v>1.3362637120549066</v>
+        <v>1.3190032340862445</v>
       </c>
       <c r="I18" s="17">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.23238842122852266</v>
+        <v>0.24914091039802716</v>
       </c>
       <c r="J18" s="17">
         <f t="shared" ca="1" si="8"/>
-        <v>1.8053289415348868</v>
+        <v>1.3190032340862445</v>
       </c>
       <c r="K18" s="17">
         <f t="shared" ca="1" si="9"/>
-        <v>-4.1853335779117016</v>
+        <v>3.8872268891989674</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="16">
+      <c r="A19" s="17">
         <f t="shared" ca="1" si="2"/>
-        <v>184</v>
-      </c>
-      <c r="B19" s="16">
+        <v>162.00718263632467</v>
+      </c>
+      <c r="B19" s="17">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>232.83618675483763</v>
       </c>
       <c r="C19" s="17">
         <f t="shared" ca="1" si="10"/>
-        <v>4.5386575096609363</v>
+        <v>7.4155412974734936E-2</v>
       </c>
       <c r="D19" s="17">
         <f t="shared" ca="1" si="4"/>
-        <v>3.2114058236695664</v>
+        <v>2.8275587488836527</v>
       </c>
       <c r="E19" s="17">
         <f t="shared" ca="1" si="5"/>
-        <v>260.04591995892832</v>
-      </c>
-      <c r="F19" s="16">
+        <v>4.2487921915019768</v>
+      </c>
+      <c r="F19" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>162.00718263632467</v>
       </c>
       <c r="G19" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>0.97658438329062935</v>
+        <v>-0.97694203763691945</v>
       </c>
       <c r="H19" s="17">
         <f t="shared" ca="1" si="7"/>
-        <v>1.3539665617978009</v>
+        <v>-1.3556353503445775</v>
       </c>
       <c r="I19" s="17">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.21513470736462095</v>
+        <v>0.21350469572780806</v>
       </c>
       <c r="J19" s="17">
         <f t="shared" ca="1" si="8"/>
-        <v>1.7876260917919922</v>
+        <v>1.3556353503445768</v>
       </c>
       <c r="K19" s="17">
         <f t="shared" ca="1" si="9"/>
-        <v>-4.53940879764912</v>
+        <v>-4.575740286679217</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="16">
+      <c r="A20" s="17">
         <f t="shared" ca="1" si="2"/>
-        <v>213</v>
-      </c>
-      <c r="B20" s="16">
+        <v>234.90555503484239</v>
+      </c>
+      <c r="B20" s="17">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>57.163272243788697</v>
       </c>
       <c r="C20" s="17">
         <f t="shared" ca="1" si="10"/>
-        <v>4.873545590400588</v>
+        <v>6.6538049018356045</v>
       </c>
       <c r="D20" s="17">
         <f t="shared" ca="1" si="4"/>
-        <v>3.717551306747922</v>
+        <v>4.0998753665827428</v>
       </c>
       <c r="E20" s="17">
         <f t="shared" ca="1" si="5"/>
-        <v>279.23359359454668</v>
-      </c>
-      <c r="F20" s="16">
+        <v>381.23493857863917</v>
+      </c>
+      <c r="F20" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>6.252466059687606</v>
       </c>
       <c r="G20" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>-0.58777061981984058</v>
+        <v>0.65478187095851814</v>
       </c>
       <c r="H20" s="17">
         <f t="shared" ca="1" si="7"/>
-        <v>-0.62830044410594033</v>
+        <v>0.71389398439209928</v>
       </c>
       <c r="I20" s="17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.80902762528643013</v>
+        <v>-0.75581790231778878</v>
       </c>
       <c r="J20" s="17">
         <f t="shared" ca="1" si="8"/>
-        <v>0.62830044410594021</v>
+        <v>2.4276986691976941</v>
       </c>
       <c r="K20" s="17">
         <f t="shared" ca="1" si="9"/>
-        <v>-0.72651489448428264</v>
+        <v>-0.86632225692268761</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="16">
+      <c r="A21" s="17">
         <f t="shared" ca="1" si="2"/>
-        <v>200</v>
-      </c>
-      <c r="B21" s="16">
+        <v>276.9843256647186</v>
+      </c>
+      <c r="B21" s="17">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>190.50948118423307</v>
       </c>
       <c r="C21" s="17">
         <f t="shared" ca="1" si="10"/>
-        <v>6.7414954723928293</v>
+        <v>3.7838084607000906</v>
       </c>
       <c r="D21" s="17">
         <f t="shared" ca="1" si="4"/>
-        <v>3.4906585039886591</v>
+        <v>4.8342884592655713</v>
       </c>
       <c r="E21" s="17">
         <f t="shared" ca="1" si="5"/>
-        <v>386.2592381746623</v>
-      </c>
-      <c r="F21" s="16">
+        <v>216.7962552840078</v>
+      </c>
+      <c r="F21" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>86.47484448048553</v>
       </c>
       <c r="G21" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>-0.87329729721399463</v>
+        <v>0.50049647355664706</v>
       </c>
       <c r="H21" s="17">
         <f t="shared" ca="1" si="7"/>
-        <v>-1.0619298297467676</v>
+        <v>0.52417214881679164</v>
       </c>
       <c r="I21" s="17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.48718767500700588</v>
+        <v>0.8657385748350136</v>
       </c>
       <c r="J21" s="17">
         <f t="shared" ca="1" si="8"/>
-        <v>1.0619298297467674</v>
+        <v>0.52417214881679164</v>
       </c>
       <c r="K21" s="17">
         <f t="shared" ca="1" si="9"/>
-        <v>-1.7925274837903817</v>
+        <v>0.57811502005906135</v>
       </c>
     </row>
   </sheetData>
@@ -6848,351 +6847,351 @@
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="21">
         <f ca="1">$A$2 + RANDBETWEEN(1, NOW() - $A$2)</f>
-        <v>4306.03125</v>
+        <v>14715.03125</v>
       </c>
       <c r="B3" s="23">
         <f t="shared" ref="B3:B37" ca="1" si="0">A3</f>
-        <v>4306.03125</v>
+        <v>14715.03125</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="21">
         <f t="shared" ref="A4:A37" ca="1" si="1">$A$2 + RANDBETWEEN(1, NOW() - $A$2)</f>
-        <v>7987.03125</v>
+        <v>1583.03125</v>
       </c>
       <c r="B4" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>7987.03125</v>
+        <v>1583.03125</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>2636.03125</v>
+        <v>39219.03125</v>
       </c>
       <c r="B5" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>2636.03125</v>
+        <v>39219.03125</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>11200.03125</v>
+        <v>37340.03125</v>
       </c>
       <c r="B6" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>11200.03125</v>
+        <v>37340.03125</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>28869.03125</v>
+        <v>7192.03125</v>
       </c>
       <c r="B7" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>28869.03125</v>
+        <v>7192.03125</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>32894.03125</v>
+        <v>31890.03125</v>
       </c>
       <c r="B8" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>32894.03125</v>
+        <v>31890.03125</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>32441.03125</v>
+        <v>33189.03125</v>
       </c>
       <c r="B9" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>32441.03125</v>
+        <v>33189.03125</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>6382.03125</v>
+        <v>1451.03125</v>
       </c>
       <c r="B10" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>6382.03125</v>
+        <v>1451.03125</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>14230.03125</v>
+        <v>1285.03125</v>
       </c>
       <c r="B11" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>14230.03125</v>
+        <v>1285.03125</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>8840.03125</v>
+        <v>30202.03125</v>
       </c>
       <c r="B12" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>8840.03125</v>
+        <v>30202.03125</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>35155.03125</v>
+        <v>36495.03125</v>
       </c>
       <c r="B13" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>35155.03125</v>
+        <v>36495.03125</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>22983.03125</v>
+        <v>32159.03125</v>
       </c>
       <c r="B14" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>22983.03125</v>
+        <v>32159.03125</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>4270.03125</v>
+        <v>25248.03125</v>
       </c>
       <c r="B15" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>4270.03125</v>
+        <v>25248.03125</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>8037.03125</v>
+        <v>38923.03125</v>
       </c>
       <c r="B16" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>8037.03125</v>
+        <v>38923.03125</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>25286.03125</v>
+        <v>22162.03125</v>
       </c>
       <c r="B17" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>25286.03125</v>
+        <v>22162.03125</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>27187.03125</v>
+        <v>1496.03125</v>
       </c>
       <c r="B18" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>27187.03125</v>
+        <v>1496.03125</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>32212.03125</v>
+        <v>9379.03125</v>
       </c>
       <c r="B19" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>32212.03125</v>
+        <v>9379.03125</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>22981.03125</v>
+        <v>41353.03125</v>
       </c>
       <c r="B20" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>22981.03125</v>
+        <v>41353.03125</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>7805.03125</v>
+        <v>14356.03125</v>
       </c>
       <c r="B21" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>7805.03125</v>
+        <v>14356.03125</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>21675.03125</v>
+        <v>27695.03125</v>
       </c>
       <c r="B22" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>21675.03125</v>
+        <v>27695.03125</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>587.03125</v>
+        <v>38874.03125</v>
       </c>
       <c r="B23" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>587.03125</v>
+        <v>38874.03125</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>8175.03125</v>
+        <v>12612.03125</v>
       </c>
       <c r="B24" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>8175.03125</v>
+        <v>12612.03125</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>23737.03125</v>
+        <v>33454.03125</v>
       </c>
       <c r="B25" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>23737.03125</v>
+        <v>33454.03125</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>40293.03125</v>
+        <v>4222.03125</v>
       </c>
       <c r="B26" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>40293.03125</v>
+        <v>4222.03125</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>8984.03125</v>
+        <v>10411.03125</v>
       </c>
       <c r="B27" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>8984.03125</v>
+        <v>10411.03125</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>13827.03125</v>
+        <v>25231.03125</v>
       </c>
       <c r="B28" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>13827.03125</v>
+        <v>25231.03125</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>29844.03125</v>
+        <v>32073.03125</v>
       </c>
       <c r="B29" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>29844.03125</v>
+        <v>32073.03125</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>37014.03125</v>
+        <v>1623.03125</v>
       </c>
       <c r="B30" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>37014.03125</v>
+        <v>1623.03125</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>19911.03125</v>
+        <v>27142.03125</v>
       </c>
       <c r="B31" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>19911.03125</v>
+        <v>27142.03125</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>13449.03125</v>
+        <v>6812.03125</v>
       </c>
       <c r="B32" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>13449.03125</v>
+        <v>6812.03125</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>35763.03125</v>
+        <v>33031.03125</v>
       </c>
       <c r="B33" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>35763.03125</v>
+        <v>33031.03125</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>28000.03125</v>
+        <v>27608.03125</v>
       </c>
       <c r="B34" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>28000.03125</v>
+        <v>27608.03125</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>34634.03125</v>
+        <v>36591.03125</v>
       </c>
       <c r="B35" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>34634.03125</v>
+        <v>36591.03125</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>5419.03125</v>
+        <v>22249.03125</v>
       </c>
       <c r="B36" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>5419.03125</v>
+        <v>22249.03125</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>2152.03125</v>
+        <v>18006.03125</v>
       </c>
       <c r="B37" s="23">
         <f t="shared" ca="1" si="0"/>
-        <v>2152.03125</v>
+        <v>18006.03125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>